<commit_message>
Add new flag images for CD, DO, and GE in 60x40 pixel format
- Added cd_60x40.png to flags_cache
- Added do_60x40.png to flags_cache
- Added ge_60x40.png to flags_cache
</commit_message>
<xml_diff>
--- a/data/3FEB_25_26/clutch_lineups_25_26_3FEB.xlsx
+++ b/data/3FEB_25_26/clutch_lineups_25_26_3FEB.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:X157"/>
+  <dimension ref="A1:X193"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -13121,6 +13121,2926 @@
         </is>
       </c>
     </row>
+    <row r="158">
+      <c r="A158" t="n">
+        <v>2487638</v>
+      </c>
+      <c r="B158" t="inlineStr">
+        <is>
+          <t>CB ARIDANE</t>
+        </is>
+      </c>
+      <c r="C158" t="inlineStr">
+        <is>
+          <t>A. GASE SECO | D. VIERA LOPEZ | K. SKUTYELNIK | O. BALSELLS PLAZA | S. GUEYE</t>
+        </is>
+      </c>
+      <c r="D158" t="n">
+        <v>5</v>
+      </c>
+      <c r="E158" t="n">
+        <v>108</v>
+      </c>
+      <c r="F158" t="n">
+        <v>1.8</v>
+      </c>
+      <c r="G158" t="n">
+        <v>3</v>
+      </c>
+      <c r="H158" t="n">
+        <v>3</v>
+      </c>
+      <c r="I158" t="n">
+        <v>5.44</v>
+      </c>
+      <c r="J158" t="n">
+        <v>1.88</v>
+      </c>
+      <c r="K158" t="n">
+        <v>55.15</v>
+      </c>
+      <c r="L158" t="n">
+        <v>159.57</v>
+      </c>
+      <c r="M158" t="n">
+        <v>-104.43</v>
+      </c>
+      <c r="N158" t="n">
+        <v>4</v>
+      </c>
+      <c r="O158" t="n">
+        <v>1</v>
+      </c>
+      <c r="P158" t="n">
+        <v>2</v>
+      </c>
+      <c r="Q158" t="n">
+        <v>1</v>
+      </c>
+      <c r="R158" t="n">
+        <v>2</v>
+      </c>
+      <c r="S158" t="n">
+        <v>2</v>
+      </c>
+      <c r="T158" t="n">
+        <v>1</v>
+      </c>
+      <c r="U158" t="n">
+        <v>2</v>
+      </c>
+      <c r="V158" t="inlineStr">
+        <is>
+          <t>Liga Regular "B-B"</t>
+        </is>
+      </c>
+      <c r="W158" t="n">
+        <v>9</v>
+      </c>
+      <c r="X158" t="inlineStr">
+        <is>
+          <t>RECUCYM BAZU vs CB ARIDANE</t>
+        </is>
+      </c>
+    </row>
+    <row r="159">
+      <c r="A159" t="n">
+        <v>2487638</v>
+      </c>
+      <c r="B159" t="inlineStr">
+        <is>
+          <t>CB ARIDANE</t>
+        </is>
+      </c>
+      <c r="C159" t="inlineStr">
+        <is>
+          <t>A. GASE SECO | D. VIERA LOPEZ | J. ABRIL RAMIRO | O. BALSELLS PLAZA | S. GUEYE</t>
+        </is>
+      </c>
+      <c r="D159" t="n">
+        <v>5</v>
+      </c>
+      <c r="E159" t="n">
+        <v>99</v>
+      </c>
+      <c r="F159" t="n">
+        <v>1.65</v>
+      </c>
+      <c r="G159" t="n">
+        <v>3</v>
+      </c>
+      <c r="H159" t="n">
+        <v>3</v>
+      </c>
+      <c r="I159" t="n">
+        <v>2</v>
+      </c>
+      <c r="J159" t="n">
+        <v>1.88</v>
+      </c>
+      <c r="K159" t="n">
+        <v>150</v>
+      </c>
+      <c r="L159" t="n">
+        <v>159.57</v>
+      </c>
+      <c r="M159" t="n">
+        <v>-9.57</v>
+      </c>
+      <c r="N159" t="n">
+        <v>3</v>
+      </c>
+      <c r="O159" t="n">
+        <v>0</v>
+      </c>
+      <c r="P159" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q159" t="n">
+        <v>1</v>
+      </c>
+      <c r="R159" t="n">
+        <v>2</v>
+      </c>
+      <c r="S159" t="n">
+        <v>2</v>
+      </c>
+      <c r="T159" t="n">
+        <v>0</v>
+      </c>
+      <c r="U159" t="n">
+        <v>1</v>
+      </c>
+      <c r="V159" t="inlineStr">
+        <is>
+          <t>Liga Regular "B-B"</t>
+        </is>
+      </c>
+      <c r="W159" t="n">
+        <v>9</v>
+      </c>
+      <c r="X159" t="inlineStr">
+        <is>
+          <t>RECUCYM BAZU vs CB ARIDANE</t>
+        </is>
+      </c>
+    </row>
+    <row r="160">
+      <c r="A160" t="n">
+        <v>2487638</v>
+      </c>
+      <c r="B160" t="inlineStr">
+        <is>
+          <t>CB ARIDANE</t>
+        </is>
+      </c>
+      <c r="C160" t="inlineStr">
+        <is>
+          <t>A. GASE SECO | D. VIERA LOPEZ | J. LARREA IBARBURU | K. SKUTYELNIK | O. BALSELLS PLAZA</t>
+        </is>
+      </c>
+      <c r="D160" t="n">
+        <v>5</v>
+      </c>
+      <c r="E160" t="n">
+        <v>78</v>
+      </c>
+      <c r="F160" t="n">
+        <v>1.3</v>
+      </c>
+      <c r="G160" t="n">
+        <v>1</v>
+      </c>
+      <c r="H160" t="n">
+        <v>6</v>
+      </c>
+      <c r="I160" t="n">
+        <v>2.88</v>
+      </c>
+      <c r="J160" t="n">
+        <v>2.52</v>
+      </c>
+      <c r="K160" t="n">
+        <v>34.72</v>
+      </c>
+      <c r="L160" t="n">
+        <v>238.1</v>
+      </c>
+      <c r="M160" t="n">
+        <v>-203.37</v>
+      </c>
+      <c r="N160" t="n">
+        <v>2</v>
+      </c>
+      <c r="O160" t="n">
+        <v>2</v>
+      </c>
+      <c r="P160" t="n">
+        <v>1</v>
+      </c>
+      <c r="Q160" t="n">
+        <v>1</v>
+      </c>
+      <c r="R160" t="n">
+        <v>0</v>
+      </c>
+      <c r="S160" t="n">
+        <v>8</v>
+      </c>
+      <c r="T160" t="n">
+        <v>0</v>
+      </c>
+      <c r="U160" t="n">
+        <v>1</v>
+      </c>
+      <c r="V160" t="inlineStr">
+        <is>
+          <t>Liga Regular "B-B"</t>
+        </is>
+      </c>
+      <c r="W160" t="n">
+        <v>9</v>
+      </c>
+      <c r="X160" t="inlineStr">
+        <is>
+          <t>RECUCYM BAZU vs CB ARIDANE</t>
+        </is>
+      </c>
+    </row>
+    <row r="161">
+      <c r="A161" t="n">
+        <v>2487638</v>
+      </c>
+      <c r="B161" t="inlineStr">
+        <is>
+          <t>RECUCYM BAZU</t>
+        </is>
+      </c>
+      <c r="C161" t="inlineStr">
+        <is>
+          <t>G. HIERRO ABAD | J. BARRA DE LA CRUZ | L. DE LA CRUZ DE LA ROSA | M. OILLATAGUERRE | V. FERNANDEZ MORAN</t>
+        </is>
+      </c>
+      <c r="D161" t="n">
+        <v>5</v>
+      </c>
+      <c r="E161" t="n">
+        <v>184</v>
+      </c>
+      <c r="F161" t="n">
+        <v>3.07</v>
+      </c>
+      <c r="G161" t="n">
+        <v>6</v>
+      </c>
+      <c r="H161" t="n">
+        <v>6</v>
+      </c>
+      <c r="I161" t="n">
+        <v>3.76</v>
+      </c>
+      <c r="J161" t="n">
+        <v>6.44</v>
+      </c>
+      <c r="K161" t="n">
+        <v>159.57</v>
+      </c>
+      <c r="L161" t="n">
+        <v>93.17</v>
+      </c>
+      <c r="M161" t="n">
+        <v>66.41</v>
+      </c>
+      <c r="N161" t="n">
+        <v>3</v>
+      </c>
+      <c r="O161" t="n">
+        <v>4</v>
+      </c>
+      <c r="P161" t="n">
+        <v>1</v>
+      </c>
+      <c r="Q161" t="n">
+        <v>2</v>
+      </c>
+      <c r="R161" t="n">
+        <v>6</v>
+      </c>
+      <c r="S161" t="n">
+        <v>1</v>
+      </c>
+      <c r="T161" t="n">
+        <v>2</v>
+      </c>
+      <c r="U161" t="n">
+        <v>2</v>
+      </c>
+      <c r="V161" t="inlineStr">
+        <is>
+          <t>Liga Regular "B-B"</t>
+        </is>
+      </c>
+      <c r="W161" t="n">
+        <v>9</v>
+      </c>
+      <c r="X161" t="inlineStr">
+        <is>
+          <t>RECUCYM BAZU vs CB ARIDANE</t>
+        </is>
+      </c>
+    </row>
+    <row r="162">
+      <c r="A162" t="n">
+        <v>2487638</v>
+      </c>
+      <c r="B162" t="inlineStr">
+        <is>
+          <t>RECUCYM BAZU</t>
+        </is>
+      </c>
+      <c r="C162" t="inlineStr">
+        <is>
+          <t>G. HIERRO ABAD | J. BARRA DE LA CRUZ | J. MUNRO | L. DE LA CRUZ DE LA ROSA | M. OILLATAGUERRE</t>
+        </is>
+      </c>
+      <c r="D162" t="n">
+        <v>5</v>
+      </c>
+      <c r="E162" t="n">
+        <v>78</v>
+      </c>
+      <c r="F162" t="n">
+        <v>1.3</v>
+      </c>
+      <c r="G162" t="n">
+        <v>6</v>
+      </c>
+      <c r="H162" t="n">
+        <v>1</v>
+      </c>
+      <c r="I162" t="n">
+        <v>2.52</v>
+      </c>
+      <c r="J162" t="n">
+        <v>2.88</v>
+      </c>
+      <c r="K162" t="n">
+        <v>238.1</v>
+      </c>
+      <c r="L162" t="n">
+        <v>34.72</v>
+      </c>
+      <c r="M162" t="n">
+        <v>203.37</v>
+      </c>
+      <c r="N162" t="n">
+        <v>0</v>
+      </c>
+      <c r="O162" t="n">
+        <v>8</v>
+      </c>
+      <c r="P162" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q162" t="n">
+        <v>1</v>
+      </c>
+      <c r="R162" t="n">
+        <v>2</v>
+      </c>
+      <c r="S162" t="n">
+        <v>2</v>
+      </c>
+      <c r="T162" t="n">
+        <v>1</v>
+      </c>
+      <c r="U162" t="n">
+        <v>1</v>
+      </c>
+      <c r="V162" t="inlineStr">
+        <is>
+          <t>Liga Regular "B-B"</t>
+        </is>
+      </c>
+      <c r="W162" t="n">
+        <v>9</v>
+      </c>
+      <c r="X162" t="inlineStr">
+        <is>
+          <t>RECUCYM BAZU vs CB ARIDANE</t>
+        </is>
+      </c>
+    </row>
+    <row r="163">
+      <c r="A163" t="n">
+        <v>2487638</v>
+      </c>
+      <c r="B163" t="inlineStr">
+        <is>
+          <t>RECUCYM BAZU</t>
+        </is>
+      </c>
+      <c r="C163" t="inlineStr">
+        <is>
+          <t>J. BARRA DE LA CRUZ | J. MENDOZA ALVAREZ | L. DE LA CRUZ DE LA ROSA | M. OILLATAGUERRE | V. FERNANDEZ MORAN</t>
+        </is>
+      </c>
+      <c r="D163" t="n">
+        <v>5</v>
+      </c>
+      <c r="E163" t="n">
+        <v>23</v>
+      </c>
+      <c r="F163" t="n">
+        <v>0.38</v>
+      </c>
+      <c r="G163" t="n">
+        <v>0</v>
+      </c>
+      <c r="H163" t="n">
+        <v>0</v>
+      </c>
+      <c r="I163" t="n">
+        <v>0</v>
+      </c>
+      <c r="J163" t="n">
+        <v>1</v>
+      </c>
+      <c r="K163" t="inlineStr"/>
+      <c r="L163" t="n">
+        <v>0</v>
+      </c>
+      <c r="M163" t="inlineStr"/>
+      <c r="N163" t="n">
+        <v>1</v>
+      </c>
+      <c r="O163" t="n">
+        <v>0</v>
+      </c>
+      <c r="P163" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q163" t="n">
+        <v>1</v>
+      </c>
+      <c r="R163" t="n">
+        <v>1</v>
+      </c>
+      <c r="S163" t="n">
+        <v>0</v>
+      </c>
+      <c r="T163" t="n">
+        <v>0</v>
+      </c>
+      <c r="U163" t="n">
+        <v>0</v>
+      </c>
+      <c r="V163" t="inlineStr">
+        <is>
+          <t>Liga Regular "B-B"</t>
+        </is>
+      </c>
+      <c r="W163" t="n">
+        <v>9</v>
+      </c>
+      <c r="X163" t="inlineStr">
+        <is>
+          <t>RECUCYM BAZU vs CB ARIDANE</t>
+        </is>
+      </c>
+    </row>
+    <row r="164">
+      <c r="A164" t="n">
+        <v>2487635</v>
+      </c>
+      <c r="B164" t="inlineStr">
+        <is>
+          <t>EB FELIPE ANTÓN</t>
+        </is>
+      </c>
+      <c r="C164" t="inlineStr">
+        <is>
+          <t>A. SISTAC RODRIGUEZ | B. FERNANDEZ SHEPHARD | M. NIMAGA | P. ARGÜELLES ELORZA | P. HERNANDEZ RODRIGUEZ</t>
+        </is>
+      </c>
+      <c r="D164" t="n">
+        <v>5</v>
+      </c>
+      <c r="E164" t="n">
+        <v>98</v>
+      </c>
+      <c r="F164" t="n">
+        <v>1.63</v>
+      </c>
+      <c r="G164" t="n">
+        <v>2</v>
+      </c>
+      <c r="H164" t="n">
+        <v>0</v>
+      </c>
+      <c r="I164" t="n">
+        <v>3</v>
+      </c>
+      <c r="J164" t="n">
+        <v>1</v>
+      </c>
+      <c r="K164" t="n">
+        <v>66.67</v>
+      </c>
+      <c r="L164" t="n">
+        <v>0</v>
+      </c>
+      <c r="M164" t="n">
+        <v>66.67</v>
+      </c>
+      <c r="N164" t="n">
+        <v>4</v>
+      </c>
+      <c r="O164" t="n">
+        <v>0</v>
+      </c>
+      <c r="P164" t="n">
+        <v>1</v>
+      </c>
+      <c r="Q164" t="n">
+        <v>2</v>
+      </c>
+      <c r="R164" t="n">
+        <v>2</v>
+      </c>
+      <c r="S164" t="n">
+        <v>0</v>
+      </c>
+      <c r="T164" t="n">
+        <v>1</v>
+      </c>
+      <c r="U164" t="n">
+        <v>2</v>
+      </c>
+      <c r="V164" t="inlineStr">
+        <is>
+          <t>Liga Regular "B-B"</t>
+        </is>
+      </c>
+      <c r="W164" t="n">
+        <v>9</v>
+      </c>
+      <c r="X164" t="inlineStr">
+        <is>
+          <t>EB FELIPE ANTÓN vs GRUPO EGIDO PINTOBASKET</t>
+        </is>
+      </c>
+    </row>
+    <row r="165">
+      <c r="A165" t="n">
+        <v>2487635</v>
+      </c>
+      <c r="B165" t="inlineStr">
+        <is>
+          <t>EB FELIPE ANTÓN</t>
+        </is>
+      </c>
+      <c r="C165" t="inlineStr">
+        <is>
+          <t>A. SISTAC RODRIGUEZ | E. DUQUE NEGRÍN | M. NIMAGA | P. ARGÜELLES ELORZA | S. MANERO GUZMAN</t>
+        </is>
+      </c>
+      <c r="D165" t="n">
+        <v>5</v>
+      </c>
+      <c r="E165" t="n">
+        <v>64</v>
+      </c>
+      <c r="F165" t="n">
+        <v>1.07</v>
+      </c>
+      <c r="G165" t="n">
+        <v>3</v>
+      </c>
+      <c r="H165" t="n">
+        <v>0</v>
+      </c>
+      <c r="I165" t="n">
+        <v>1.76</v>
+      </c>
+      <c r="J165" t="n">
+        <v>2</v>
+      </c>
+      <c r="K165" t="n">
+        <v>170.45</v>
+      </c>
+      <c r="L165" t="n">
+        <v>0</v>
+      </c>
+      <c r="M165" t="n">
+        <v>170.45</v>
+      </c>
+      <c r="N165" t="n">
+        <v>1</v>
+      </c>
+      <c r="O165" t="n">
+        <v>4</v>
+      </c>
+      <c r="P165" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q165" t="n">
+        <v>1</v>
+      </c>
+      <c r="R165" t="n">
+        <v>1</v>
+      </c>
+      <c r="S165" t="n">
+        <v>0</v>
+      </c>
+      <c r="T165" t="n">
+        <v>1</v>
+      </c>
+      <c r="U165" t="n">
+        <v>0</v>
+      </c>
+      <c r="V165" t="inlineStr">
+        <is>
+          <t>Liga Regular "B-B"</t>
+        </is>
+      </c>
+      <c r="W165" t="n">
+        <v>9</v>
+      </c>
+      <c r="X165" t="inlineStr">
+        <is>
+          <t>EB FELIPE ANTÓN vs GRUPO EGIDO PINTOBASKET</t>
+        </is>
+      </c>
+    </row>
+    <row r="166">
+      <c r="A166" t="n">
+        <v>2487635</v>
+      </c>
+      <c r="B166" t="inlineStr">
+        <is>
+          <t>EB FELIPE ANTÓN</t>
+        </is>
+      </c>
+      <c r="C166" t="inlineStr">
+        <is>
+          <t>A. SISTAC RODRIGUEZ | B. FERNANDEZ SHEPHARD | E. DUQUE NEGRÍN | M. NIMAGA | S. MANERO GUZMAN</t>
+        </is>
+      </c>
+      <c r="D166" t="n">
+        <v>5</v>
+      </c>
+      <c r="E166" t="n">
+        <v>25</v>
+      </c>
+      <c r="F166" t="n">
+        <v>0.42</v>
+      </c>
+      <c r="G166" t="n">
+        <v>0</v>
+      </c>
+      <c r="H166" t="n">
+        <v>0</v>
+      </c>
+      <c r="I166" t="n">
+        <v>-1</v>
+      </c>
+      <c r="J166" t="n">
+        <v>0.88</v>
+      </c>
+      <c r="K166" t="inlineStr"/>
+      <c r="L166" t="n">
+        <v>0</v>
+      </c>
+      <c r="M166" t="inlineStr"/>
+      <c r="N166" t="n">
+        <v>0</v>
+      </c>
+      <c r="O166" t="n">
+        <v>0</v>
+      </c>
+      <c r="P166" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q166" t="n">
+        <v>1</v>
+      </c>
+      <c r="R166" t="n">
+        <v>0</v>
+      </c>
+      <c r="S166" t="n">
+        <v>2</v>
+      </c>
+      <c r="T166" t="n">
+        <v>0</v>
+      </c>
+      <c r="U166" t="n">
+        <v>0</v>
+      </c>
+      <c r="V166" t="inlineStr">
+        <is>
+          <t>Liga Regular "B-B"</t>
+        </is>
+      </c>
+      <c r="W166" t="n">
+        <v>9</v>
+      </c>
+      <c r="X166" t="inlineStr">
+        <is>
+          <t>EB FELIPE ANTÓN vs GRUPO EGIDO PINTOBASKET</t>
+        </is>
+      </c>
+    </row>
+    <row r="167">
+      <c r="A167" t="n">
+        <v>2487635</v>
+      </c>
+      <c r="B167" t="inlineStr">
+        <is>
+          <t>EB FELIPE ANTÓN</t>
+        </is>
+      </c>
+      <c r="C167" t="inlineStr">
+        <is>
+          <t>A. SISTAC RODRIGUEZ | B. FERNANDEZ SHEPHARD | M. NIMAGA | P. HERNANDEZ RODRIGUEZ | S. MANERO GUZMAN</t>
+        </is>
+      </c>
+      <c r="D167" t="n">
+        <v>5</v>
+      </c>
+      <c r="E167" t="n">
+        <v>14</v>
+      </c>
+      <c r="F167" t="n">
+        <v>0.23</v>
+      </c>
+      <c r="G167" t="n">
+        <v>3</v>
+      </c>
+      <c r="H167" t="n">
+        <v>0</v>
+      </c>
+      <c r="I167" t="n">
+        <v>2.44</v>
+      </c>
+      <c r="J167" t="n">
+        <v>0</v>
+      </c>
+      <c r="K167" t="n">
+        <v>122.95</v>
+      </c>
+      <c r="L167" t="inlineStr"/>
+      <c r="M167" t="inlineStr"/>
+      <c r="N167" t="n">
+        <v>2</v>
+      </c>
+      <c r="O167" t="n">
+        <v>1</v>
+      </c>
+      <c r="P167" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q167" t="n">
+        <v>0</v>
+      </c>
+      <c r="R167" t="n">
+        <v>0</v>
+      </c>
+      <c r="S167" t="n">
+        <v>0</v>
+      </c>
+      <c r="T167" t="n">
+        <v>0</v>
+      </c>
+      <c r="U167" t="n">
+        <v>0</v>
+      </c>
+      <c r="V167" t="inlineStr">
+        <is>
+          <t>Liga Regular "B-B"</t>
+        </is>
+      </c>
+      <c r="W167" t="n">
+        <v>9</v>
+      </c>
+      <c r="X167" t="inlineStr">
+        <is>
+          <t>EB FELIPE ANTÓN vs GRUPO EGIDO PINTOBASKET</t>
+        </is>
+      </c>
+    </row>
+    <row r="168">
+      <c r="A168" t="n">
+        <v>2487635</v>
+      </c>
+      <c r="B168" t="inlineStr">
+        <is>
+          <t>EB FELIPE ANTÓN</t>
+        </is>
+      </c>
+      <c r="C168" t="inlineStr">
+        <is>
+          <t>A. SISTAC RODRIGUEZ | E. DUQUE NEGRÍN | K. RIVEROL DE LAS CASAS | P. ARGÜELLES ELORZA | S. MANERO GUZMAN</t>
+        </is>
+      </c>
+      <c r="D168" t="n">
+        <v>5</v>
+      </c>
+      <c r="E168" t="n">
+        <v>12</v>
+      </c>
+      <c r="F168" t="n">
+        <v>0.2</v>
+      </c>
+      <c r="G168" t="n">
+        <v>0</v>
+      </c>
+      <c r="H168" t="n">
+        <v>0</v>
+      </c>
+      <c r="I168" t="n">
+        <v>1</v>
+      </c>
+      <c r="J168" t="n">
+        <v>0</v>
+      </c>
+      <c r="K168" t="n">
+        <v>0</v>
+      </c>
+      <c r="L168" t="inlineStr"/>
+      <c r="M168" t="inlineStr"/>
+      <c r="N168" t="n">
+        <v>1</v>
+      </c>
+      <c r="O168" t="n">
+        <v>0</v>
+      </c>
+      <c r="P168" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q168" t="n">
+        <v>0</v>
+      </c>
+      <c r="R168" t="n">
+        <v>0</v>
+      </c>
+      <c r="S168" t="n">
+        <v>0</v>
+      </c>
+      <c r="T168" t="n">
+        <v>0</v>
+      </c>
+      <c r="U168" t="n">
+        <v>0</v>
+      </c>
+      <c r="V168" t="inlineStr">
+        <is>
+          <t>Liga Regular "B-B"</t>
+        </is>
+      </c>
+      <c r="W168" t="n">
+        <v>9</v>
+      </c>
+      <c r="X168" t="inlineStr">
+        <is>
+          <t>EB FELIPE ANTÓN vs GRUPO EGIDO PINTOBASKET</t>
+        </is>
+      </c>
+    </row>
+    <row r="169">
+      <c r="A169" t="n">
+        <v>2487635</v>
+      </c>
+      <c r="B169" t="inlineStr">
+        <is>
+          <t>EB FELIPE ANTÓN</t>
+        </is>
+      </c>
+      <c r="C169" t="inlineStr">
+        <is>
+          <t>A. SISTAC RODRIGUEZ | K. RIVEROL DE LAS CASAS | M. NIMAGA | P. ARGÜELLES ELORZA | P. HERNANDEZ RODRIGUEZ</t>
+        </is>
+      </c>
+      <c r="D169" t="n">
+        <v>5</v>
+      </c>
+      <c r="E169" t="n">
+        <v>11</v>
+      </c>
+      <c r="F169" t="n">
+        <v>0.18</v>
+      </c>
+      <c r="G169" t="n">
+        <v>0</v>
+      </c>
+      <c r="H169" t="n">
+        <v>0</v>
+      </c>
+      <c r="I169" t="n">
+        <v>-1</v>
+      </c>
+      <c r="J169" t="n">
+        <v>1</v>
+      </c>
+      <c r="K169" t="inlineStr"/>
+      <c r="L169" t="n">
+        <v>0</v>
+      </c>
+      <c r="M169" t="inlineStr"/>
+      <c r="N169" t="n">
+        <v>0</v>
+      </c>
+      <c r="O169" t="n">
+        <v>0</v>
+      </c>
+      <c r="P169" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q169" t="n">
+        <v>1</v>
+      </c>
+      <c r="R169" t="n">
+        <v>1</v>
+      </c>
+      <c r="S169" t="n">
+        <v>0</v>
+      </c>
+      <c r="T169" t="n">
+        <v>0</v>
+      </c>
+      <c r="U169" t="n">
+        <v>0</v>
+      </c>
+      <c r="V169" t="inlineStr">
+        <is>
+          <t>Liga Regular "B-B"</t>
+        </is>
+      </c>
+      <c r="W169" t="n">
+        <v>9</v>
+      </c>
+      <c r="X169" t="inlineStr">
+        <is>
+          <t>EB FELIPE ANTÓN vs GRUPO EGIDO PINTOBASKET</t>
+        </is>
+      </c>
+    </row>
+    <row r="170">
+      <c r="A170" t="n">
+        <v>2487635</v>
+      </c>
+      <c r="B170" t="inlineStr">
+        <is>
+          <t>GRUPO EGIDO PINTOBASKET</t>
+        </is>
+      </c>
+      <c r="C170" t="inlineStr">
+        <is>
+          <t>D. TOLOSA OROPESA | F. SANTAMARIA LEON | J. AYALA AYLLÓN | M. ALARCON ORTIZ | M. BATLLE BERNARDO</t>
+        </is>
+      </c>
+      <c r="D170" t="n">
+        <v>5</v>
+      </c>
+      <c r="E170" t="n">
+        <v>143</v>
+      </c>
+      <c r="F170" t="n">
+        <v>2.38</v>
+      </c>
+      <c r="G170" t="n">
+        <v>0</v>
+      </c>
+      <c r="H170" t="n">
+        <v>5</v>
+      </c>
+      <c r="I170" t="n">
+        <v>2.88</v>
+      </c>
+      <c r="J170" t="n">
+        <v>3.44</v>
+      </c>
+      <c r="K170" t="n">
+        <v>0</v>
+      </c>
+      <c r="L170" t="n">
+        <v>145.35</v>
+      </c>
+      <c r="M170" t="n">
+        <v>-145.35</v>
+      </c>
+      <c r="N170" t="n">
+        <v>3</v>
+      </c>
+      <c r="O170" t="n">
+        <v>2</v>
+      </c>
+      <c r="P170" t="n">
+        <v>1</v>
+      </c>
+      <c r="Q170" t="n">
+        <v>2</v>
+      </c>
+      <c r="R170" t="n">
+        <v>6</v>
+      </c>
+      <c r="S170" t="n">
+        <v>1</v>
+      </c>
+      <c r="T170" t="n">
+        <v>1</v>
+      </c>
+      <c r="U170" t="n">
+        <v>4</v>
+      </c>
+      <c r="V170" t="inlineStr">
+        <is>
+          <t>Liga Regular "B-B"</t>
+        </is>
+      </c>
+      <c r="W170" t="n">
+        <v>9</v>
+      </c>
+      <c r="X170" t="inlineStr">
+        <is>
+          <t>EB FELIPE ANTÓN vs GRUPO EGIDO PINTOBASKET</t>
+        </is>
+      </c>
+    </row>
+    <row r="171">
+      <c r="A171" t="n">
+        <v>2487635</v>
+      </c>
+      <c r="B171" t="inlineStr">
+        <is>
+          <t>GRUPO EGIDO PINTOBASKET</t>
+        </is>
+      </c>
+      <c r="C171" t="inlineStr">
+        <is>
+          <t>D. TOLOSA OROPESA | F. SANTAMARIA LEON | J. TRUJILLO FERNÁNDEZ | M. ALARCON ORTIZ | M. BATLLE BERNARDO</t>
+        </is>
+      </c>
+      <c r="D171" t="n">
+        <v>5</v>
+      </c>
+      <c r="E171" t="n">
+        <v>60</v>
+      </c>
+      <c r="F171" t="n">
+        <v>1</v>
+      </c>
+      <c r="G171" t="n">
+        <v>0</v>
+      </c>
+      <c r="H171" t="n">
+        <v>1</v>
+      </c>
+      <c r="I171" t="n">
+        <v>2</v>
+      </c>
+      <c r="J171" t="n">
+        <v>1.88</v>
+      </c>
+      <c r="K171" t="n">
+        <v>0</v>
+      </c>
+      <c r="L171" t="n">
+        <v>53.19</v>
+      </c>
+      <c r="M171" t="n">
+        <v>-53.19</v>
+      </c>
+      <c r="N171" t="n">
+        <v>1</v>
+      </c>
+      <c r="O171" t="n">
+        <v>0</v>
+      </c>
+      <c r="P171" t="n">
+        <v>1</v>
+      </c>
+      <c r="Q171" t="n">
+        <v>0</v>
+      </c>
+      <c r="R171" t="n">
+        <v>2</v>
+      </c>
+      <c r="S171" t="n">
+        <v>2</v>
+      </c>
+      <c r="T171" t="n">
+        <v>0</v>
+      </c>
+      <c r="U171" t="n">
+        <v>1</v>
+      </c>
+      <c r="V171" t="inlineStr">
+        <is>
+          <t>Liga Regular "B-B"</t>
+        </is>
+      </c>
+      <c r="W171" t="n">
+        <v>9</v>
+      </c>
+      <c r="X171" t="inlineStr">
+        <is>
+          <t>EB FELIPE ANTÓN vs GRUPO EGIDO PINTOBASKET</t>
+        </is>
+      </c>
+    </row>
+    <row r="172">
+      <c r="A172" t="n">
+        <v>2487635</v>
+      </c>
+      <c r="B172" t="inlineStr">
+        <is>
+          <t>GRUPO EGIDO PINTOBASKET</t>
+        </is>
+      </c>
+      <c r="C172" t="inlineStr">
+        <is>
+          <t>D. TOLOSA OROPESA | F. SANTAMARIA LEON | M. ALARCON ORTIZ | M. BATLLE BERNARDO | M. SANZ CÁMARA</t>
+        </is>
+      </c>
+      <c r="D172" t="n">
+        <v>5</v>
+      </c>
+      <c r="E172" t="n">
+        <v>21</v>
+      </c>
+      <c r="F172" t="n">
+        <v>0.35</v>
+      </c>
+      <c r="G172" t="n">
+        <v>0</v>
+      </c>
+      <c r="H172" t="n">
+        <v>2</v>
+      </c>
+      <c r="I172" t="n">
+        <v>0</v>
+      </c>
+      <c r="J172" t="n">
+        <v>0.88</v>
+      </c>
+      <c r="K172" t="inlineStr"/>
+      <c r="L172" t="n">
+        <v>227.27</v>
+      </c>
+      <c r="M172" t="inlineStr"/>
+      <c r="N172" t="n">
+        <v>0</v>
+      </c>
+      <c r="O172" t="n">
+        <v>0</v>
+      </c>
+      <c r="P172" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q172" t="n">
+        <v>0</v>
+      </c>
+      <c r="R172" t="n">
+        <v>0</v>
+      </c>
+      <c r="S172" t="n">
+        <v>2</v>
+      </c>
+      <c r="T172" t="n">
+        <v>0</v>
+      </c>
+      <c r="U172" t="n">
+        <v>0</v>
+      </c>
+      <c r="V172" t="inlineStr">
+        <is>
+          <t>Liga Regular "B-B"</t>
+        </is>
+      </c>
+      <c r="W172" t="n">
+        <v>9</v>
+      </c>
+      <c r="X172" t="inlineStr">
+        <is>
+          <t>EB FELIPE ANTÓN vs GRUPO EGIDO PINTOBASKET</t>
+        </is>
+      </c>
+    </row>
+    <row r="173">
+      <c r="A173" t="n">
+        <v>2487645</v>
+      </c>
+      <c r="B173" t="inlineStr">
+        <is>
+          <t>C. D. MENSAJERO ISLA DE LA PALMA</t>
+        </is>
+      </c>
+      <c r="C173" t="inlineStr">
+        <is>
+          <t>D. RODRIGUEZ GARCIA | I. REBERGEN | M. NIANG | M. RODRÍGUEZ RIVEROL | P. RODRIGUEZ RIVERO</t>
+        </is>
+      </c>
+      <c r="D173" t="n">
+        <v>5</v>
+      </c>
+      <c r="E173" t="n">
+        <v>118</v>
+      </c>
+      <c r="F173" t="n">
+        <v>1.97</v>
+      </c>
+      <c r="G173" t="n">
+        <v>6</v>
+      </c>
+      <c r="H173" t="n">
+        <v>3</v>
+      </c>
+      <c r="I173" t="n">
+        <v>2</v>
+      </c>
+      <c r="J173" t="n">
+        <v>4.32</v>
+      </c>
+      <c r="K173" t="n">
+        <v>300</v>
+      </c>
+      <c r="L173" t="n">
+        <v>69.44</v>
+      </c>
+      <c r="M173" t="n">
+        <v>230.56</v>
+      </c>
+      <c r="N173" t="n">
+        <v>3</v>
+      </c>
+      <c r="O173" t="n">
+        <v>0</v>
+      </c>
+      <c r="P173" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q173" t="n">
+        <v>1</v>
+      </c>
+      <c r="R173" t="n">
+        <v>3</v>
+      </c>
+      <c r="S173" t="n">
+        <v>3</v>
+      </c>
+      <c r="T173" t="n">
+        <v>0</v>
+      </c>
+      <c r="U173" t="n">
+        <v>0</v>
+      </c>
+      <c r="V173" t="inlineStr">
+        <is>
+          <t>Liga Regular "B-B"</t>
+        </is>
+      </c>
+      <c r="W173" t="n">
+        <v>10</v>
+      </c>
+      <c r="X173" t="inlineStr">
+        <is>
+          <t>C. D. MENSAJERO ISLA DE LA PALMA vs EB FELIPE ANTÓN</t>
+        </is>
+      </c>
+    </row>
+    <row r="174">
+      <c r="A174" t="n">
+        <v>2487645</v>
+      </c>
+      <c r="B174" t="inlineStr">
+        <is>
+          <t>C. D. MENSAJERO ISLA DE LA PALMA</t>
+        </is>
+      </c>
+      <c r="C174" t="inlineStr">
+        <is>
+          <t>A. APARICIO IZQUIERDO | D. RODRIGUEZ GARCIA | I. REBERGEN | M. NIANG | P. RODRIGUEZ RIVERO</t>
+        </is>
+      </c>
+      <c r="D174" t="n">
+        <v>5</v>
+      </c>
+      <c r="E174" t="n">
+        <v>99</v>
+      </c>
+      <c r="F174" t="n">
+        <v>1.65</v>
+      </c>
+      <c r="G174" t="n">
+        <v>5</v>
+      </c>
+      <c r="H174" t="n">
+        <v>3</v>
+      </c>
+      <c r="I174" t="n">
+        <v>3.88</v>
+      </c>
+      <c r="J174" t="n">
+        <v>4</v>
+      </c>
+      <c r="K174" t="n">
+        <v>128.87</v>
+      </c>
+      <c r="L174" t="n">
+        <v>75</v>
+      </c>
+      <c r="M174" t="n">
+        <v>53.87</v>
+      </c>
+      <c r="N174" t="n">
+        <v>1</v>
+      </c>
+      <c r="O174" t="n">
+        <v>2</v>
+      </c>
+      <c r="P174" t="n">
+        <v>2</v>
+      </c>
+      <c r="Q174" t="n">
+        <v>0</v>
+      </c>
+      <c r="R174" t="n">
+        <v>3</v>
+      </c>
+      <c r="S174" t="n">
+        <v>0</v>
+      </c>
+      <c r="T174" t="n">
+        <v>2</v>
+      </c>
+      <c r="U174" t="n">
+        <v>1</v>
+      </c>
+      <c r="V174" t="inlineStr">
+        <is>
+          <t>Liga Regular "B-B"</t>
+        </is>
+      </c>
+      <c r="W174" t="n">
+        <v>10</v>
+      </c>
+      <c r="X174" t="inlineStr">
+        <is>
+          <t>C. D. MENSAJERO ISLA DE LA PALMA vs EB FELIPE ANTÓN</t>
+        </is>
+      </c>
+    </row>
+    <row r="175">
+      <c r="A175" t="n">
+        <v>2487645</v>
+      </c>
+      <c r="B175" t="inlineStr">
+        <is>
+          <t>C. D. MENSAJERO ISLA DE LA PALMA</t>
+        </is>
+      </c>
+      <c r="C175" t="inlineStr">
+        <is>
+          <t>I. REBERGEN | M. NIANG | M. RODRÍGUEZ RIVEROL | O. PEÑA LOPEZ | P. RODRIGUEZ RIVERO</t>
+        </is>
+      </c>
+      <c r="D175" t="n">
+        <v>5</v>
+      </c>
+      <c r="E175" t="n">
+        <v>30</v>
+      </c>
+      <c r="F175" t="n">
+        <v>0.5</v>
+      </c>
+      <c r="G175" t="n">
+        <v>0</v>
+      </c>
+      <c r="H175" t="n">
+        <v>2</v>
+      </c>
+      <c r="I175" t="n">
+        <v>1</v>
+      </c>
+      <c r="J175" t="n">
+        <v>1</v>
+      </c>
+      <c r="K175" t="n">
+        <v>0</v>
+      </c>
+      <c r="L175" t="n">
+        <v>200</v>
+      </c>
+      <c r="M175" t="n">
+        <v>-200</v>
+      </c>
+      <c r="N175" t="n">
+        <v>0</v>
+      </c>
+      <c r="O175" t="n">
+        <v>0</v>
+      </c>
+      <c r="P175" t="n">
+        <v>1</v>
+      </c>
+      <c r="Q175" t="n">
+        <v>0</v>
+      </c>
+      <c r="R175" t="n">
+        <v>1</v>
+      </c>
+      <c r="S175" t="n">
+        <v>0</v>
+      </c>
+      <c r="T175" t="n">
+        <v>0</v>
+      </c>
+      <c r="U175" t="n">
+        <v>0</v>
+      </c>
+      <c r="V175" t="inlineStr">
+        <is>
+          <t>Liga Regular "B-B"</t>
+        </is>
+      </c>
+      <c r="W175" t="n">
+        <v>10</v>
+      </c>
+      <c r="X175" t="inlineStr">
+        <is>
+          <t>C. D. MENSAJERO ISLA DE LA PALMA vs EB FELIPE ANTÓN</t>
+        </is>
+      </c>
+    </row>
+    <row r="176">
+      <c r="A176" t="n">
+        <v>2487645</v>
+      </c>
+      <c r="B176" t="inlineStr">
+        <is>
+          <t>C. D. MENSAJERO ISLA DE LA PALMA</t>
+        </is>
+      </c>
+      <c r="C176" t="inlineStr">
+        <is>
+          <t>A. APARICIO IZQUIERDO | D. RODRIGUEZ GARCIA | I. REBERGEN | J. RIES | P. RODRIGUEZ RIVERO</t>
+        </is>
+      </c>
+      <c r="D176" t="n">
+        <v>5</v>
+      </c>
+      <c r="E176" t="n">
+        <v>2</v>
+      </c>
+      <c r="F176" t="n">
+        <v>0.03</v>
+      </c>
+      <c r="G176" t="n">
+        <v>3</v>
+      </c>
+      <c r="H176" t="n">
+        <v>0</v>
+      </c>
+      <c r="I176" t="n">
+        <v>1.44</v>
+      </c>
+      <c r="J176" t="n">
+        <v>0</v>
+      </c>
+      <c r="K176" t="n">
+        <v>208.33</v>
+      </c>
+      <c r="L176" t="inlineStr"/>
+      <c r="M176" t="inlineStr"/>
+      <c r="N176" t="n">
+        <v>1</v>
+      </c>
+      <c r="O176" t="n">
+        <v>1</v>
+      </c>
+      <c r="P176" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q176" t="n">
+        <v>0</v>
+      </c>
+      <c r="R176" t="n">
+        <v>0</v>
+      </c>
+      <c r="S176" t="n">
+        <v>0</v>
+      </c>
+      <c r="T176" t="n">
+        <v>0</v>
+      </c>
+      <c r="U176" t="n">
+        <v>0</v>
+      </c>
+      <c r="V176" t="inlineStr">
+        <is>
+          <t>Liga Regular "B-B"</t>
+        </is>
+      </c>
+      <c r="W176" t="n">
+        <v>10</v>
+      </c>
+      <c r="X176" t="inlineStr">
+        <is>
+          <t>C. D. MENSAJERO ISLA DE LA PALMA vs EB FELIPE ANTÓN</t>
+        </is>
+      </c>
+    </row>
+    <row r="177">
+      <c r="A177" t="n">
+        <v>2487645</v>
+      </c>
+      <c r="B177" t="inlineStr">
+        <is>
+          <t>EB FELIPE ANTÓN</t>
+        </is>
+      </c>
+      <c r="C177" t="inlineStr">
+        <is>
+          <t>A. SISTAC RODRIGUEZ | B. FERNANDEZ SHEPHARD | E. DUQUE NEGRÍN | M. NIMAGA | S. MANERO GUZMAN</t>
+        </is>
+      </c>
+      <c r="D177" t="n">
+        <v>5</v>
+      </c>
+      <c r="E177" t="n">
+        <v>118</v>
+      </c>
+      <c r="F177" t="n">
+        <v>1.97</v>
+      </c>
+      <c r="G177" t="n">
+        <v>3</v>
+      </c>
+      <c r="H177" t="n">
+        <v>6</v>
+      </c>
+      <c r="I177" t="n">
+        <v>4.32</v>
+      </c>
+      <c r="J177" t="n">
+        <v>2</v>
+      </c>
+      <c r="K177" t="n">
+        <v>69.44</v>
+      </c>
+      <c r="L177" t="n">
+        <v>300</v>
+      </c>
+      <c r="M177" t="n">
+        <v>-230.56</v>
+      </c>
+      <c r="N177" t="n">
+        <v>3</v>
+      </c>
+      <c r="O177" t="n">
+        <v>3</v>
+      </c>
+      <c r="P177" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q177" t="n">
+        <v>0</v>
+      </c>
+      <c r="R177" t="n">
+        <v>3</v>
+      </c>
+      <c r="S177" t="n">
+        <v>0</v>
+      </c>
+      <c r="T177" t="n">
+        <v>0</v>
+      </c>
+      <c r="U177" t="n">
+        <v>1</v>
+      </c>
+      <c r="V177" t="inlineStr">
+        <is>
+          <t>Liga Regular "B-B"</t>
+        </is>
+      </c>
+      <c r="W177" t="n">
+        <v>10</v>
+      </c>
+      <c r="X177" t="inlineStr">
+        <is>
+          <t>C. D. MENSAJERO ISLA DE LA PALMA vs EB FELIPE ANTÓN</t>
+        </is>
+      </c>
+    </row>
+    <row r="178">
+      <c r="A178" t="n">
+        <v>2487645</v>
+      </c>
+      <c r="B178" t="inlineStr">
+        <is>
+          <t>EB FELIPE ANTÓN</t>
+        </is>
+      </c>
+      <c r="C178" t="inlineStr">
+        <is>
+          <t>E. DUQUE NEGRÍN | J. GALLETTO LAMELA | M. NIMAGA | P. ARGÜELLES ELORZA | S. MANERO GUZMAN</t>
+        </is>
+      </c>
+      <c r="D178" t="n">
+        <v>5</v>
+      </c>
+      <c r="E178" t="n">
+        <v>98</v>
+      </c>
+      <c r="F178" t="n">
+        <v>1.63</v>
+      </c>
+      <c r="G178" t="n">
+        <v>3</v>
+      </c>
+      <c r="H178" t="n">
+        <v>3</v>
+      </c>
+      <c r="I178" t="n">
+        <v>3</v>
+      </c>
+      <c r="J178" t="n">
+        <v>3</v>
+      </c>
+      <c r="K178" t="n">
+        <v>100</v>
+      </c>
+      <c r="L178" t="n">
+        <v>100</v>
+      </c>
+      <c r="M178" t="n">
+        <v>0</v>
+      </c>
+      <c r="N178" t="n">
+        <v>3</v>
+      </c>
+      <c r="O178" t="n">
+        <v>0</v>
+      </c>
+      <c r="P178" t="n">
+        <v>1</v>
+      </c>
+      <c r="Q178" t="n">
+        <v>1</v>
+      </c>
+      <c r="R178" t="n">
+        <v>1</v>
+      </c>
+      <c r="S178" t="n">
+        <v>0</v>
+      </c>
+      <c r="T178" t="n">
+        <v>2</v>
+      </c>
+      <c r="U178" t="n">
+        <v>0</v>
+      </c>
+      <c r="V178" t="inlineStr">
+        <is>
+          <t>Liga Regular "B-B"</t>
+        </is>
+      </c>
+      <c r="W178" t="n">
+        <v>10</v>
+      </c>
+      <c r="X178" t="inlineStr">
+        <is>
+          <t>C. D. MENSAJERO ISLA DE LA PALMA vs EB FELIPE ANTÓN</t>
+        </is>
+      </c>
+    </row>
+    <row r="179">
+      <c r="A179" t="n">
+        <v>2487645</v>
+      </c>
+      <c r="B179" t="inlineStr">
+        <is>
+          <t>EB FELIPE ANTÓN</t>
+        </is>
+      </c>
+      <c r="C179" t="inlineStr">
+        <is>
+          <t>A. SISTAC RODRIGUEZ | E. DUQUE NEGRÍN | K. RIVEROL DE LAS CASAS | M. NIMAGA | S. MANERO GUZMAN</t>
+        </is>
+      </c>
+      <c r="D179" t="n">
+        <v>5</v>
+      </c>
+      <c r="E179" t="n">
+        <v>30</v>
+      </c>
+      <c r="F179" t="n">
+        <v>0.5</v>
+      </c>
+      <c r="G179" t="n">
+        <v>2</v>
+      </c>
+      <c r="H179" t="n">
+        <v>0</v>
+      </c>
+      <c r="I179" t="n">
+        <v>1</v>
+      </c>
+      <c r="J179" t="n">
+        <v>1</v>
+      </c>
+      <c r="K179" t="n">
+        <v>200</v>
+      </c>
+      <c r="L179" t="n">
+        <v>0</v>
+      </c>
+      <c r="M179" t="n">
+        <v>200</v>
+      </c>
+      <c r="N179" t="n">
+        <v>1</v>
+      </c>
+      <c r="O179" t="n">
+        <v>0</v>
+      </c>
+      <c r="P179" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q179" t="n">
+        <v>0</v>
+      </c>
+      <c r="R179" t="n">
+        <v>0</v>
+      </c>
+      <c r="S179" t="n">
+        <v>0</v>
+      </c>
+      <c r="T179" t="n">
+        <v>1</v>
+      </c>
+      <c r="U179" t="n">
+        <v>0</v>
+      </c>
+      <c r="V179" t="inlineStr">
+        <is>
+          <t>Liga Regular "B-B"</t>
+        </is>
+      </c>
+      <c r="W179" t="n">
+        <v>10</v>
+      </c>
+      <c r="X179" t="inlineStr">
+        <is>
+          <t>C. D. MENSAJERO ISLA DE LA PALMA vs EB FELIPE ANTÓN</t>
+        </is>
+      </c>
+    </row>
+    <row r="180">
+      <c r="A180" t="n">
+        <v>2487645</v>
+      </c>
+      <c r="B180" t="inlineStr">
+        <is>
+          <t>EB FELIPE ANTÓN</t>
+        </is>
+      </c>
+      <c r="C180" t="inlineStr">
+        <is>
+          <t>E. DUQUE NEGRÍN | J. GALLETTO LAMELA | K. RIVEROL DE LAS CASAS | M. NIMAGA | S. MANERO GUZMAN</t>
+        </is>
+      </c>
+      <c r="D180" t="n">
+        <v>5</v>
+      </c>
+      <c r="E180" t="n">
+        <v>3</v>
+      </c>
+      <c r="F180" t="n">
+        <v>0.05</v>
+      </c>
+      <c r="G180" t="n">
+        <v>0</v>
+      </c>
+      <c r="H180" t="n">
+        <v>5</v>
+      </c>
+      <c r="I180" t="n">
+        <v>1</v>
+      </c>
+      <c r="J180" t="n">
+        <v>2.32</v>
+      </c>
+      <c r="K180" t="n">
+        <v>0</v>
+      </c>
+      <c r="L180" t="n">
+        <v>215.52</v>
+      </c>
+      <c r="M180" t="n">
+        <v>-215.52</v>
+      </c>
+      <c r="N180" t="n">
+        <v>0</v>
+      </c>
+      <c r="O180" t="n">
+        <v>0</v>
+      </c>
+      <c r="P180" t="n">
+        <v>1</v>
+      </c>
+      <c r="Q180" t="n">
+        <v>0</v>
+      </c>
+      <c r="R180" t="n">
+        <v>1</v>
+      </c>
+      <c r="S180" t="n">
+        <v>3</v>
+      </c>
+      <c r="T180" t="n">
+        <v>0</v>
+      </c>
+      <c r="U180" t="n">
+        <v>0</v>
+      </c>
+      <c r="V180" t="inlineStr">
+        <is>
+          <t>Liga Regular "B-B"</t>
+        </is>
+      </c>
+      <c r="W180" t="n">
+        <v>10</v>
+      </c>
+      <c r="X180" t="inlineStr">
+        <is>
+          <t>C. D. MENSAJERO ISLA DE LA PALMA vs EB FELIPE ANTÓN</t>
+        </is>
+      </c>
+    </row>
+    <row r="181">
+      <c r="A181" t="n">
+        <v>2487643</v>
+      </c>
+      <c r="B181" t="inlineStr">
+        <is>
+          <t>ADC BOADILLA</t>
+        </is>
+      </c>
+      <c r="C181" t="inlineStr">
+        <is>
+          <t>A. GOMEZ SERRANO | A. OLMEDO VELASCO | I. BLANCO-ARGIBAY GONZALEZ | M. SANCHEZ SANCHEZ | P. DOMINGUEZ LORENZO</t>
+        </is>
+      </c>
+      <c r="D181" t="n">
+        <v>5</v>
+      </c>
+      <c r="E181" t="n">
+        <v>320</v>
+      </c>
+      <c r="F181" t="n">
+        <v>5.33</v>
+      </c>
+      <c r="G181" t="n">
+        <v>9</v>
+      </c>
+      <c r="H181" t="n">
+        <v>14</v>
+      </c>
+      <c r="I181" t="n">
+        <v>6.88</v>
+      </c>
+      <c r="J181" t="n">
+        <v>7.76</v>
+      </c>
+      <c r="K181" t="n">
+        <v>130.81</v>
+      </c>
+      <c r="L181" t="n">
+        <v>180.41</v>
+      </c>
+      <c r="M181" t="n">
+        <v>-49.6</v>
+      </c>
+      <c r="N181" t="n">
+        <v>9</v>
+      </c>
+      <c r="O181" t="n">
+        <v>2</v>
+      </c>
+      <c r="P181" t="n">
+        <v>1</v>
+      </c>
+      <c r="Q181" t="n">
+        <v>4</v>
+      </c>
+      <c r="R181" t="n">
+        <v>10</v>
+      </c>
+      <c r="S181" t="n">
+        <v>4</v>
+      </c>
+      <c r="T181" t="n">
+        <v>0</v>
+      </c>
+      <c r="U181" t="n">
+        <v>4</v>
+      </c>
+      <c r="V181" t="inlineStr">
+        <is>
+          <t>Liga Regular "B-B"</t>
+        </is>
+      </c>
+      <c r="W181" t="n">
+        <v>10</v>
+      </c>
+      <c r="X181" t="inlineStr">
+        <is>
+          <t>AUTOCARES RODRÍGUEZ vs ADC BOADILLA</t>
+        </is>
+      </c>
+    </row>
+    <row r="182">
+      <c r="A182" t="n">
+        <v>2487643</v>
+      </c>
+      <c r="B182" t="inlineStr">
+        <is>
+          <t>ADC BOADILLA</t>
+        </is>
+      </c>
+      <c r="C182" t="inlineStr">
+        <is>
+          <t>A. OLMEDO VELASCO | E. BOADA MONTESDEOCA | E. PEREZ BERNABEU | H. SANTANA DE LA ROSA | I. BLANCO-ARGIBAY GONZALEZ</t>
+        </is>
+      </c>
+      <c r="D182" t="n">
+        <v>5</v>
+      </c>
+      <c r="E182" t="n">
+        <v>199</v>
+      </c>
+      <c r="F182" t="n">
+        <v>3.32</v>
+      </c>
+      <c r="G182" t="n">
+        <v>7</v>
+      </c>
+      <c r="H182" t="n">
+        <v>12</v>
+      </c>
+      <c r="I182" t="n">
+        <v>4.88</v>
+      </c>
+      <c r="J182" t="n">
+        <v>6.76</v>
+      </c>
+      <c r="K182" t="n">
+        <v>143.44</v>
+      </c>
+      <c r="L182" t="n">
+        <v>177.51</v>
+      </c>
+      <c r="M182" t="n">
+        <v>-34.07</v>
+      </c>
+      <c r="N182" t="n">
+        <v>3</v>
+      </c>
+      <c r="O182" t="n">
+        <v>2</v>
+      </c>
+      <c r="P182" t="n">
+        <v>2</v>
+      </c>
+      <c r="Q182" t="n">
+        <v>1</v>
+      </c>
+      <c r="R182" t="n">
+        <v>5</v>
+      </c>
+      <c r="S182" t="n">
+        <v>4</v>
+      </c>
+      <c r="T182" t="n">
+        <v>0</v>
+      </c>
+      <c r="U182" t="n">
+        <v>0</v>
+      </c>
+      <c r="V182" t="inlineStr">
+        <is>
+          <t>Liga Regular "B-B"</t>
+        </is>
+      </c>
+      <c r="W182" t="n">
+        <v>10</v>
+      </c>
+      <c r="X182" t="inlineStr">
+        <is>
+          <t>AUTOCARES RODRÍGUEZ vs ADC BOADILLA</t>
+        </is>
+      </c>
+    </row>
+    <row r="183">
+      <c r="A183" t="n">
+        <v>2487643</v>
+      </c>
+      <c r="B183" t="inlineStr">
+        <is>
+          <t>ADC BOADILLA</t>
+        </is>
+      </c>
+      <c r="C183" t="inlineStr">
+        <is>
+          <t>A. OLMEDO VELASCO | E. BOADA MONTESDEOCA | E. PEREZ BERNABEU | I. BLANCO-ARGIBAY GONZALEZ | P. DOMINGUEZ LORENZO</t>
+        </is>
+      </c>
+      <c r="D183" t="n">
+        <v>5</v>
+      </c>
+      <c r="E183" t="n">
+        <v>157</v>
+      </c>
+      <c r="F183" t="n">
+        <v>2.62</v>
+      </c>
+      <c r="G183" t="n">
+        <v>3</v>
+      </c>
+      <c r="H183" t="n">
+        <v>0</v>
+      </c>
+      <c r="I183" t="n">
+        <v>4.76</v>
+      </c>
+      <c r="J183" t="n">
+        <v>4.76</v>
+      </c>
+      <c r="K183" t="n">
+        <v>63.03</v>
+      </c>
+      <c r="L183" t="n">
+        <v>0</v>
+      </c>
+      <c r="M183" t="n">
+        <v>63.03</v>
+      </c>
+      <c r="N183" t="n">
+        <v>3</v>
+      </c>
+      <c r="O183" t="n">
+        <v>4</v>
+      </c>
+      <c r="P183" t="n">
+        <v>2</v>
+      </c>
+      <c r="Q183" t="n">
+        <v>2</v>
+      </c>
+      <c r="R183" t="n">
+        <v>3</v>
+      </c>
+      <c r="S183" t="n">
+        <v>4</v>
+      </c>
+      <c r="T183" t="n">
+        <v>4</v>
+      </c>
+      <c r="U183" t="n">
+        <v>4</v>
+      </c>
+      <c r="V183" t="inlineStr">
+        <is>
+          <t>Liga Regular "B-B"</t>
+        </is>
+      </c>
+      <c r="W183" t="n">
+        <v>10</v>
+      </c>
+      <c r="X183" t="inlineStr">
+        <is>
+          <t>AUTOCARES RODRÍGUEZ vs ADC BOADILLA</t>
+        </is>
+      </c>
+    </row>
+    <row r="184">
+      <c r="A184" t="n">
+        <v>2487643</v>
+      </c>
+      <c r="B184" t="inlineStr">
+        <is>
+          <t>ADC BOADILLA</t>
+        </is>
+      </c>
+      <c r="C184" t="inlineStr">
+        <is>
+          <t>A. GOMEZ SERRANO | A. OLMEDO VELASCO | E. BOADA MONTESDEOCA | E. PEREZ BERNABEU | P. DOMINGUEZ LORENZO</t>
+        </is>
+      </c>
+      <c r="D184" t="n">
+        <v>5</v>
+      </c>
+      <c r="E184" t="n">
+        <v>131</v>
+      </c>
+      <c r="F184" t="n">
+        <v>2.18</v>
+      </c>
+      <c r="G184" t="n">
+        <v>0</v>
+      </c>
+      <c r="H184" t="n">
+        <v>5</v>
+      </c>
+      <c r="I184" t="n">
+        <v>5</v>
+      </c>
+      <c r="J184" t="n">
+        <v>4.88</v>
+      </c>
+      <c r="K184" t="n">
+        <v>0</v>
+      </c>
+      <c r="L184" t="n">
+        <v>102.46</v>
+      </c>
+      <c r="M184" t="n">
+        <v>-102.46</v>
+      </c>
+      <c r="N184" t="n">
+        <v>2</v>
+      </c>
+      <c r="O184" t="n">
+        <v>0</v>
+      </c>
+      <c r="P184" t="n">
+        <v>3</v>
+      </c>
+      <c r="Q184" t="n">
+        <v>0</v>
+      </c>
+      <c r="R184" t="n">
+        <v>5</v>
+      </c>
+      <c r="S184" t="n">
+        <v>2</v>
+      </c>
+      <c r="T184" t="n">
+        <v>0</v>
+      </c>
+      <c r="U184" t="n">
+        <v>1</v>
+      </c>
+      <c r="V184" t="inlineStr">
+        <is>
+          <t>Liga Regular "B-B"</t>
+        </is>
+      </c>
+      <c r="W184" t="n">
+        <v>10</v>
+      </c>
+      <c r="X184" t="inlineStr">
+        <is>
+          <t>AUTOCARES RODRÍGUEZ vs ADC BOADILLA</t>
+        </is>
+      </c>
+    </row>
+    <row r="185">
+      <c r="A185" t="n">
+        <v>2487643</v>
+      </c>
+      <c r="B185" t="inlineStr">
+        <is>
+          <t>ADC BOADILLA</t>
+        </is>
+      </c>
+      <c r="C185" t="inlineStr">
+        <is>
+          <t>A. GOMEZ SERRANO | A. OLMEDO VELASCO | E. BOADA MONTESDEOCA | I. BLANCO-ARGIBAY GONZALEZ | P. DOMINGUEZ LORENZO</t>
+        </is>
+      </c>
+      <c r="D185" t="n">
+        <v>5</v>
+      </c>
+      <c r="E185" t="n">
+        <v>54</v>
+      </c>
+      <c r="F185" t="n">
+        <v>0.9</v>
+      </c>
+      <c r="G185" t="n">
+        <v>2</v>
+      </c>
+      <c r="H185" t="n">
+        <v>3</v>
+      </c>
+      <c r="I185" t="n">
+        <v>0.88</v>
+      </c>
+      <c r="J185" t="n">
+        <v>0.88</v>
+      </c>
+      <c r="K185" t="n">
+        <v>227.27</v>
+      </c>
+      <c r="L185" t="n">
+        <v>340.91</v>
+      </c>
+      <c r="M185" t="n">
+        <v>-113.64</v>
+      </c>
+      <c r="N185" t="n">
+        <v>1</v>
+      </c>
+      <c r="O185" t="n">
+        <v>2</v>
+      </c>
+      <c r="P185" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q185" t="n">
+        <v>1</v>
+      </c>
+      <c r="R185" t="n">
+        <v>1</v>
+      </c>
+      <c r="S185" t="n">
+        <v>2</v>
+      </c>
+      <c r="T185" t="n">
+        <v>0</v>
+      </c>
+      <c r="U185" t="n">
+        <v>1</v>
+      </c>
+      <c r="V185" t="inlineStr">
+        <is>
+          <t>Liga Regular "B-B"</t>
+        </is>
+      </c>
+      <c r="W185" t="n">
+        <v>10</v>
+      </c>
+      <c r="X185" t="inlineStr">
+        <is>
+          <t>AUTOCARES RODRÍGUEZ vs ADC BOADILLA</t>
+        </is>
+      </c>
+    </row>
+    <row r="186">
+      <c r="A186" t="n">
+        <v>2487643</v>
+      </c>
+      <c r="B186" t="inlineStr">
+        <is>
+          <t>ADC BOADILLA</t>
+        </is>
+      </c>
+      <c r="C186" t="inlineStr">
+        <is>
+          <t>A. OLMEDO VELASCO | E. BOADA MONTESDEOCA | E. PEREZ BERNABEU | H. SANTANA DE LA ROSA | P. DOMINGUEZ LORENZO</t>
+        </is>
+      </c>
+      <c r="D186" t="n">
+        <v>5</v>
+      </c>
+      <c r="E186" t="n">
+        <v>53</v>
+      </c>
+      <c r="F186" t="n">
+        <v>0.88</v>
+      </c>
+      <c r="G186" t="n">
+        <v>6</v>
+      </c>
+      <c r="H186" t="n">
+        <v>2</v>
+      </c>
+      <c r="I186" t="n">
+        <v>2</v>
+      </c>
+      <c r="J186" t="n">
+        <v>2</v>
+      </c>
+      <c r="K186" t="n">
+        <v>300</v>
+      </c>
+      <c r="L186" t="n">
+        <v>100</v>
+      </c>
+      <c r="M186" t="n">
+        <v>200</v>
+      </c>
+      <c r="N186" t="n">
+        <v>2</v>
+      </c>
+      <c r="O186" t="n">
+        <v>0</v>
+      </c>
+      <c r="P186" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q186" t="n">
+        <v>0</v>
+      </c>
+      <c r="R186" t="n">
+        <v>2</v>
+      </c>
+      <c r="S186" t="n">
+        <v>0</v>
+      </c>
+      <c r="T186" t="n">
+        <v>0</v>
+      </c>
+      <c r="U186" t="n">
+        <v>0</v>
+      </c>
+      <c r="V186" t="inlineStr">
+        <is>
+          <t>Liga Regular "B-B"</t>
+        </is>
+      </c>
+      <c r="W186" t="n">
+        <v>10</v>
+      </c>
+      <c r="X186" t="inlineStr">
+        <is>
+          <t>AUTOCARES RODRÍGUEZ vs ADC BOADILLA</t>
+        </is>
+      </c>
+    </row>
+    <row r="187">
+      <c r="A187" t="n">
+        <v>2487643</v>
+      </c>
+      <c r="B187" t="inlineStr">
+        <is>
+          <t>ADC BOADILLA</t>
+        </is>
+      </c>
+      <c r="C187" t="inlineStr">
+        <is>
+          <t>A. GOMEZ SERRANO | A. OLMEDO VELASCO | E. BOADA MONTESDEOCA | E. PEREZ BERNABEU | M. SANCHEZ SANCHEZ</t>
+        </is>
+      </c>
+      <c r="D187" t="n">
+        <v>5</v>
+      </c>
+      <c r="E187" t="n">
+        <v>29</v>
+      </c>
+      <c r="F187" t="n">
+        <v>0.48</v>
+      </c>
+      <c r="G187" t="n">
+        <v>3</v>
+      </c>
+      <c r="H187" t="n">
+        <v>3</v>
+      </c>
+      <c r="I187" t="n">
+        <v>3</v>
+      </c>
+      <c r="J187" t="n">
+        <v>1</v>
+      </c>
+      <c r="K187" t="n">
+        <v>100</v>
+      </c>
+      <c r="L187" t="n">
+        <v>300</v>
+      </c>
+      <c r="M187" t="n">
+        <v>-200</v>
+      </c>
+      <c r="N187" t="n">
+        <v>1</v>
+      </c>
+      <c r="O187" t="n">
+        <v>0</v>
+      </c>
+      <c r="P187" t="n">
+        <v>2</v>
+      </c>
+      <c r="Q187" t="n">
+        <v>0</v>
+      </c>
+      <c r="R187" t="n">
+        <v>1</v>
+      </c>
+      <c r="S187" t="n">
+        <v>0</v>
+      </c>
+      <c r="T187" t="n">
+        <v>0</v>
+      </c>
+      <c r="U187" t="n">
+        <v>0</v>
+      </c>
+      <c r="V187" t="inlineStr">
+        <is>
+          <t>Liga Regular "B-B"</t>
+        </is>
+      </c>
+      <c r="W187" t="n">
+        <v>10</v>
+      </c>
+      <c r="X187" t="inlineStr">
+        <is>
+          <t>AUTOCARES RODRÍGUEZ vs ADC BOADILLA</t>
+        </is>
+      </c>
+    </row>
+    <row r="188">
+      <c r="A188" t="n">
+        <v>2487643</v>
+      </c>
+      <c r="B188" t="inlineStr">
+        <is>
+          <t>ADC BOADILLA</t>
+        </is>
+      </c>
+      <c r="C188" t="inlineStr">
+        <is>
+          <t>A. GOMEZ SERRANO | A. OLMEDO VELASCO | E. BOADA MONTESDEOCA | E. PEREZ BERNABEU | I. BLANCO-ARGIBAY GONZALEZ</t>
+        </is>
+      </c>
+      <c r="D188" t="n">
+        <v>5</v>
+      </c>
+      <c r="E188" t="n">
+        <v>15</v>
+      </c>
+      <c r="F188" t="n">
+        <v>0.25</v>
+      </c>
+      <c r="G188" t="n">
+        <v>0</v>
+      </c>
+      <c r="H188" t="n">
+        <v>2</v>
+      </c>
+      <c r="I188" t="n">
+        <v>1</v>
+      </c>
+      <c r="J188" t="n">
+        <v>1</v>
+      </c>
+      <c r="K188" t="n">
+        <v>0</v>
+      </c>
+      <c r="L188" t="n">
+        <v>200</v>
+      </c>
+      <c r="M188" t="n">
+        <v>-200</v>
+      </c>
+      <c r="N188" t="n">
+        <v>0</v>
+      </c>
+      <c r="O188" t="n">
+        <v>0</v>
+      </c>
+      <c r="P188" t="n">
+        <v>1</v>
+      </c>
+      <c r="Q188" t="n">
+        <v>0</v>
+      </c>
+      <c r="R188" t="n">
+        <v>1</v>
+      </c>
+      <c r="S188" t="n">
+        <v>0</v>
+      </c>
+      <c r="T188" t="n">
+        <v>0</v>
+      </c>
+      <c r="U188" t="n">
+        <v>0</v>
+      </c>
+      <c r="V188" t="inlineStr">
+        <is>
+          <t>Liga Regular "B-B"</t>
+        </is>
+      </c>
+      <c r="W188" t="n">
+        <v>10</v>
+      </c>
+      <c r="X188" t="inlineStr">
+        <is>
+          <t>AUTOCARES RODRÍGUEZ vs ADC BOADILLA</t>
+        </is>
+      </c>
+    </row>
+    <row r="189">
+      <c r="A189" t="n">
+        <v>2487643</v>
+      </c>
+      <c r="B189" t="inlineStr">
+        <is>
+          <t>AUTOCARES RODRÍGUEZ</t>
+        </is>
+      </c>
+      <c r="C189" t="inlineStr">
+        <is>
+          <t>F. ESPINOSA | I. GARCIA GALLARDO | P. BARCALA BELTRAN | P. VILLANUEVA LAZARO</t>
+        </is>
+      </c>
+      <c r="D189" t="n">
+        <v>4</v>
+      </c>
+      <c r="E189" t="n">
+        <v>361</v>
+      </c>
+      <c r="F189" t="n">
+        <v>6.02</v>
+      </c>
+      <c r="G189" t="n">
+        <v>21</v>
+      </c>
+      <c r="H189" t="n">
+        <v>10</v>
+      </c>
+      <c r="I189" t="n">
+        <v>12.76</v>
+      </c>
+      <c r="J189" t="n">
+        <v>10.88</v>
+      </c>
+      <c r="K189" t="n">
+        <v>164.58</v>
+      </c>
+      <c r="L189" t="n">
+        <v>91.91</v>
+      </c>
+      <c r="M189" t="n">
+        <v>72.67</v>
+      </c>
+      <c r="N189" t="n">
+        <v>12</v>
+      </c>
+      <c r="O189" t="n">
+        <v>4</v>
+      </c>
+      <c r="P189" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q189" t="n">
+        <v>1</v>
+      </c>
+      <c r="R189" t="n">
+        <v>6</v>
+      </c>
+      <c r="S189" t="n">
+        <v>2</v>
+      </c>
+      <c r="T189" t="n">
+        <v>5</v>
+      </c>
+      <c r="U189" t="n">
+        <v>1</v>
+      </c>
+      <c r="V189" t="inlineStr">
+        <is>
+          <t>Liga Regular "B-B"</t>
+        </is>
+      </c>
+      <c r="W189" t="n">
+        <v>10</v>
+      </c>
+      <c r="X189" t="inlineStr">
+        <is>
+          <t>AUTOCARES RODRÍGUEZ vs ADC BOADILLA</t>
+        </is>
+      </c>
+    </row>
+    <row r="190">
+      <c r="A190" t="n">
+        <v>2487643</v>
+      </c>
+      <c r="B190" t="inlineStr">
+        <is>
+          <t>AUTOCARES RODRÍGUEZ</t>
+        </is>
+      </c>
+      <c r="C190" t="inlineStr">
+        <is>
+          <t>F. BERMEJO FAJARDO | I. GARCIA GALLARDO | P. BARCALA BELTRAN | P. VILLANUEVA LAZARO</t>
+        </is>
+      </c>
+      <c r="D190" t="n">
+        <v>4</v>
+      </c>
+      <c r="E190" t="n">
+        <v>357</v>
+      </c>
+      <c r="F190" t="n">
+        <v>5.95</v>
+      </c>
+      <c r="G190" t="n">
+        <v>7</v>
+      </c>
+      <c r="H190" t="n">
+        <v>10</v>
+      </c>
+      <c r="I190" t="n">
+        <v>9.52</v>
+      </c>
+      <c r="J190" t="n">
+        <v>7.64</v>
+      </c>
+      <c r="K190" t="n">
+        <v>73.53</v>
+      </c>
+      <c r="L190" t="n">
+        <v>130.89</v>
+      </c>
+      <c r="M190" t="n">
+        <v>-57.36</v>
+      </c>
+      <c r="N190" t="n">
+        <v>8</v>
+      </c>
+      <c r="O190" t="n">
+        <v>8</v>
+      </c>
+      <c r="P190" t="n">
+        <v>4</v>
+      </c>
+      <c r="Q190" t="n">
+        <v>6</v>
+      </c>
+      <c r="R190" t="n">
+        <v>9</v>
+      </c>
+      <c r="S190" t="n">
+        <v>6</v>
+      </c>
+      <c r="T190" t="n">
+        <v>2</v>
+      </c>
+      <c r="U190" t="n">
+        <v>6</v>
+      </c>
+      <c r="V190" t="inlineStr">
+        <is>
+          <t>Liga Regular "B-B"</t>
+        </is>
+      </c>
+      <c r="W190" t="n">
+        <v>10</v>
+      </c>
+      <c r="X190" t="inlineStr">
+        <is>
+          <t>AUTOCARES RODRÍGUEZ vs ADC BOADILLA</t>
+        </is>
+      </c>
+    </row>
+    <row r="191">
+      <c r="A191" t="n">
+        <v>2487643</v>
+      </c>
+      <c r="B191" t="inlineStr">
+        <is>
+          <t>AUTOCARES RODRÍGUEZ</t>
+        </is>
+      </c>
+      <c r="C191" t="inlineStr">
+        <is>
+          <t>D. BUHORSKYI | F. BERMEJO FAJARDO | I. GARCIA GALLARDO | P. BARCALA BELTRAN</t>
+        </is>
+      </c>
+      <c r="D191" t="n">
+        <v>4</v>
+      </c>
+      <c r="E191" t="n">
+        <v>174</v>
+      </c>
+      <c r="F191" t="n">
+        <v>2.9</v>
+      </c>
+      <c r="G191" t="n">
+        <v>10</v>
+      </c>
+      <c r="H191" t="n">
+        <v>4</v>
+      </c>
+      <c r="I191" t="n">
+        <v>3.88</v>
+      </c>
+      <c r="J191" t="n">
+        <v>4.88</v>
+      </c>
+      <c r="K191" t="n">
+        <v>257.73</v>
+      </c>
+      <c r="L191" t="n">
+        <v>81.97</v>
+      </c>
+      <c r="M191" t="n">
+        <v>175.76</v>
+      </c>
+      <c r="N191" t="n">
+        <v>6</v>
+      </c>
+      <c r="O191" t="n">
+        <v>2</v>
+      </c>
+      <c r="P191" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q191" t="n">
+        <v>3</v>
+      </c>
+      <c r="R191" t="n">
+        <v>4</v>
+      </c>
+      <c r="S191" t="n">
+        <v>2</v>
+      </c>
+      <c r="T191" t="n">
+        <v>1</v>
+      </c>
+      <c r="U191" t="n">
+        <v>1</v>
+      </c>
+      <c r="V191" t="inlineStr">
+        <is>
+          <t>Liga Regular "B-B"</t>
+        </is>
+      </c>
+      <c r="W191" t="n">
+        <v>10</v>
+      </c>
+      <c r="X191" t="inlineStr">
+        <is>
+          <t>AUTOCARES RODRÍGUEZ vs ADC BOADILLA</t>
+        </is>
+      </c>
+    </row>
+    <row r="192">
+      <c r="A192" t="n">
+        <v>2487643</v>
+      </c>
+      <c r="B192" t="inlineStr">
+        <is>
+          <t>AUTOCARES RODRÍGUEZ</t>
+        </is>
+      </c>
+      <c r="C192" t="inlineStr">
+        <is>
+          <t>D. PETIT | F. ESPINOSA | I. GARCIA GALLARDO | P. VILLANUEVA LAZARO</t>
+        </is>
+      </c>
+      <c r="D192" t="n">
+        <v>4</v>
+      </c>
+      <c r="E192" t="n">
+        <v>57</v>
+      </c>
+      <c r="F192" t="n">
+        <v>0.95</v>
+      </c>
+      <c r="G192" t="n">
+        <v>3</v>
+      </c>
+      <c r="H192" t="n">
+        <v>3</v>
+      </c>
+      <c r="I192" t="n">
+        <v>2.88</v>
+      </c>
+      <c r="J192" t="n">
+        <v>4</v>
+      </c>
+      <c r="K192" t="n">
+        <v>104.17</v>
+      </c>
+      <c r="L192" t="n">
+        <v>75</v>
+      </c>
+      <c r="M192" t="n">
+        <v>29.17</v>
+      </c>
+      <c r="N192" t="n">
+        <v>2</v>
+      </c>
+      <c r="O192" t="n">
+        <v>2</v>
+      </c>
+      <c r="P192" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q192" t="n">
+        <v>0</v>
+      </c>
+      <c r="R192" t="n">
+        <v>1</v>
+      </c>
+      <c r="S192" t="n">
+        <v>0</v>
+      </c>
+      <c r="T192" t="n">
+        <v>3</v>
+      </c>
+      <c r="U192" t="n">
+        <v>0</v>
+      </c>
+      <c r="V192" t="inlineStr">
+        <is>
+          <t>Liga Regular "B-B"</t>
+        </is>
+      </c>
+      <c r="W192" t="n">
+        <v>10</v>
+      </c>
+      <c r="X192" t="inlineStr">
+        <is>
+          <t>AUTOCARES RODRÍGUEZ vs ADC BOADILLA</t>
+        </is>
+      </c>
+    </row>
+    <row r="193">
+      <c r="A193" t="n">
+        <v>2487643</v>
+      </c>
+      <c r="B193" t="inlineStr">
+        <is>
+          <t>AUTOCARES RODRÍGUEZ</t>
+        </is>
+      </c>
+      <c r="C193" t="inlineStr">
+        <is>
+          <t>D. CARABALLO ROPERO | F. ESPINOSA | P. BARCALA BELTRAN | P. VILLANUEVA LAZARO</t>
+        </is>
+      </c>
+      <c r="D193" t="n">
+        <v>4</v>
+      </c>
+      <c r="E193" t="n">
+        <v>9</v>
+      </c>
+      <c r="F193" t="n">
+        <v>0.15</v>
+      </c>
+      <c r="G193" t="n">
+        <v>0</v>
+      </c>
+      <c r="H193" t="n">
+        <v>3</v>
+      </c>
+      <c r="I193" t="n">
+        <v>0</v>
+      </c>
+      <c r="J193" t="n">
+        <v>1</v>
+      </c>
+      <c r="K193" t="inlineStr"/>
+      <c r="L193" t="n">
+        <v>300</v>
+      </c>
+      <c r="M193" t="inlineStr"/>
+      <c r="N193" t="n">
+        <v>0</v>
+      </c>
+      <c r="O193" t="n">
+        <v>0</v>
+      </c>
+      <c r="P193" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q193" t="n">
+        <v>0</v>
+      </c>
+      <c r="R193" t="n">
+        <v>1</v>
+      </c>
+      <c r="S193" t="n">
+        <v>0</v>
+      </c>
+      <c r="T193" t="n">
+        <v>0</v>
+      </c>
+      <c r="U193" t="n">
+        <v>0</v>
+      </c>
+      <c r="V193" t="inlineStr">
+        <is>
+          <t>Liga Regular "B-B"</t>
+        </is>
+      </c>
+      <c r="W193" t="n">
+        <v>10</v>
+      </c>
+      <c r="X193" t="inlineStr">
+        <is>
+          <t>AUTOCARES RODRÍGUEZ vs ADC BOADILLA</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Add new Excel files for players and teams data for the 25-26 season
- Created players_25_26_3FEB_games.xlsx with 7638 rows of game data.
- Created teams_25_26_3FEB.xlsx with 7545 rows of team data.
</commit_message>
<xml_diff>
--- a/data/3FEB_25_26/clutch_lineups_25_26_3FEB.xlsx
+++ b/data/3FEB_25_26/clutch_lineups_25_26_3FEB.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:X193"/>
+  <dimension ref="A1:X244"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -16041,6 +16041,4110 @@
         </is>
       </c>
     </row>
+    <row r="194">
+      <c r="A194" t="n">
+        <v>2487650</v>
+      </c>
+      <c r="B194" t="inlineStr">
+        <is>
+          <t>ADC BOADILLA</t>
+        </is>
+      </c>
+      <c r="C194" t="inlineStr">
+        <is>
+          <t>A. GOMEZ SERRANO | A. OLMEDO VELASCO | I. BLANCO-ARGIBAY GONZALEZ | M. SANCHEZ SANCHEZ | P. DOMINGUEZ LORENZO</t>
+        </is>
+      </c>
+      <c r="D194" t="n">
+        <v>5</v>
+      </c>
+      <c r="E194" t="n">
+        <v>317</v>
+      </c>
+      <c r="F194" t="n">
+        <v>5.28</v>
+      </c>
+      <c r="G194" t="n">
+        <v>7</v>
+      </c>
+      <c r="H194" t="n">
+        <v>5</v>
+      </c>
+      <c r="I194" t="n">
+        <v>9</v>
+      </c>
+      <c r="J194" t="n">
+        <v>9.640000000000001</v>
+      </c>
+      <c r="K194" t="n">
+        <v>77.78</v>
+      </c>
+      <c r="L194" t="n">
+        <v>51.87</v>
+      </c>
+      <c r="M194" t="n">
+        <v>25.91</v>
+      </c>
+      <c r="N194" t="n">
+        <v>6</v>
+      </c>
+      <c r="O194" t="n">
+        <v>0</v>
+      </c>
+      <c r="P194" t="n">
+        <v>4</v>
+      </c>
+      <c r="Q194" t="n">
+        <v>1</v>
+      </c>
+      <c r="R194" t="n">
+        <v>6</v>
+      </c>
+      <c r="S194" t="n">
+        <v>6</v>
+      </c>
+      <c r="T194" t="n">
+        <v>4</v>
+      </c>
+      <c r="U194" t="n">
+        <v>3</v>
+      </c>
+      <c r="V194" t="inlineStr">
+        <is>
+          <t>Liga Regular "B-B"</t>
+        </is>
+      </c>
+      <c r="W194" t="n">
+        <v>11</v>
+      </c>
+      <c r="X194" t="inlineStr">
+        <is>
+          <t>ADC BOADILLA vs GRUPO EGIDO PINTOBASKET</t>
+        </is>
+      </c>
+    </row>
+    <row r="195">
+      <c r="A195" t="n">
+        <v>2487650</v>
+      </c>
+      <c r="B195" t="inlineStr">
+        <is>
+          <t>ADC BOADILLA</t>
+        </is>
+      </c>
+      <c r="C195" t="inlineStr">
+        <is>
+          <t>A. GOMEZ SERRANO | A. OLMEDO VELASCO | C. CUESTA DE SANTOS | I. BLANCO-ARGIBAY GONZALEZ | P. DOMINGUEZ LORENZO</t>
+        </is>
+      </c>
+      <c r="D195" t="n">
+        <v>5</v>
+      </c>
+      <c r="E195" t="n">
+        <v>202</v>
+      </c>
+      <c r="F195" t="n">
+        <v>3.37</v>
+      </c>
+      <c r="G195" t="n">
+        <v>6</v>
+      </c>
+      <c r="H195" t="n">
+        <v>6</v>
+      </c>
+      <c r="I195" t="n">
+        <v>3.2</v>
+      </c>
+      <c r="J195" t="n">
+        <v>4.76</v>
+      </c>
+      <c r="K195" t="n">
+        <v>187.5</v>
+      </c>
+      <c r="L195" t="n">
+        <v>126.05</v>
+      </c>
+      <c r="M195" t="n">
+        <v>61.45</v>
+      </c>
+      <c r="N195" t="n">
+        <v>4</v>
+      </c>
+      <c r="O195" t="n">
+        <v>5</v>
+      </c>
+      <c r="P195" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q195" t="n">
+        <v>3</v>
+      </c>
+      <c r="R195" t="n">
+        <v>6</v>
+      </c>
+      <c r="S195" t="n">
+        <v>4</v>
+      </c>
+      <c r="T195" t="n">
+        <v>0</v>
+      </c>
+      <c r="U195" t="n">
+        <v>3</v>
+      </c>
+      <c r="V195" t="inlineStr">
+        <is>
+          <t>Liga Regular "B-B"</t>
+        </is>
+      </c>
+      <c r="W195" t="n">
+        <v>11</v>
+      </c>
+      <c r="X195" t="inlineStr">
+        <is>
+          <t>ADC BOADILLA vs GRUPO EGIDO PINTOBASKET</t>
+        </is>
+      </c>
+    </row>
+    <row r="196">
+      <c r="A196" t="n">
+        <v>2487650</v>
+      </c>
+      <c r="B196" t="inlineStr">
+        <is>
+          <t>ADC BOADILLA</t>
+        </is>
+      </c>
+      <c r="C196" t="inlineStr">
+        <is>
+          <t>A. OLMEDO VELASCO | C. CUESTA DE SANTOS | E. BOADA MONTESDEOCA | I. BLANCO-ARGIBAY GONZALEZ | P. DOMINGUEZ LORENZO</t>
+        </is>
+      </c>
+      <c r="D196" t="n">
+        <v>5</v>
+      </c>
+      <c r="E196" t="n">
+        <v>178</v>
+      </c>
+      <c r="F196" t="n">
+        <v>2.97</v>
+      </c>
+      <c r="G196" t="n">
+        <v>7</v>
+      </c>
+      <c r="H196" t="n">
+        <v>2</v>
+      </c>
+      <c r="I196" t="n">
+        <v>4.76</v>
+      </c>
+      <c r="J196" t="n">
+        <v>5</v>
+      </c>
+      <c r="K196" t="n">
+        <v>147.06</v>
+      </c>
+      <c r="L196" t="n">
+        <v>40</v>
+      </c>
+      <c r="M196" t="n">
+        <v>107.06</v>
+      </c>
+      <c r="N196" t="n">
+        <v>2</v>
+      </c>
+      <c r="O196" t="n">
+        <v>4</v>
+      </c>
+      <c r="P196" t="n">
+        <v>2</v>
+      </c>
+      <c r="Q196" t="n">
+        <v>1</v>
+      </c>
+      <c r="R196" t="n">
+        <v>4</v>
+      </c>
+      <c r="S196" t="n">
+        <v>0</v>
+      </c>
+      <c r="T196" t="n">
+        <v>1</v>
+      </c>
+      <c r="U196" t="n">
+        <v>0</v>
+      </c>
+      <c r="V196" t="inlineStr">
+        <is>
+          <t>Liga Regular "B-B"</t>
+        </is>
+      </c>
+      <c r="W196" t="n">
+        <v>11</v>
+      </c>
+      <c r="X196" t="inlineStr">
+        <is>
+          <t>ADC BOADILLA vs GRUPO EGIDO PINTOBASKET</t>
+        </is>
+      </c>
+    </row>
+    <row r="197">
+      <c r="A197" t="n">
+        <v>2487650</v>
+      </c>
+      <c r="B197" t="inlineStr">
+        <is>
+          <t>ADC BOADILLA</t>
+        </is>
+      </c>
+      <c r="C197" t="inlineStr">
+        <is>
+          <t>A. GOMEZ SERRANO | A. OLMEDO VELASCO | E. BOADA MONTESDEOCA | I. VALDIVIA MERINO | P. DOMINGUEZ LORENZO</t>
+        </is>
+      </c>
+      <c r="D197" t="n">
+        <v>5</v>
+      </c>
+      <c r="E197" t="n">
+        <v>90</v>
+      </c>
+      <c r="F197" t="n">
+        <v>1.5</v>
+      </c>
+      <c r="G197" t="n">
+        <v>0</v>
+      </c>
+      <c r="H197" t="n">
+        <v>3</v>
+      </c>
+      <c r="I197" t="n">
+        <v>2</v>
+      </c>
+      <c r="J197" t="n">
+        <v>3</v>
+      </c>
+      <c r="K197" t="n">
+        <v>0</v>
+      </c>
+      <c r="L197" t="n">
+        <v>100</v>
+      </c>
+      <c r="M197" t="n">
+        <v>-100</v>
+      </c>
+      <c r="N197" t="n">
+        <v>4</v>
+      </c>
+      <c r="O197" t="n">
+        <v>0</v>
+      </c>
+      <c r="P197" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q197" t="n">
+        <v>2</v>
+      </c>
+      <c r="R197" t="n">
+        <v>3</v>
+      </c>
+      <c r="S197" t="n">
+        <v>0</v>
+      </c>
+      <c r="T197" t="n">
+        <v>1</v>
+      </c>
+      <c r="U197" t="n">
+        <v>1</v>
+      </c>
+      <c r="V197" t="inlineStr">
+        <is>
+          <t>Liga Regular "B-B"</t>
+        </is>
+      </c>
+      <c r="W197" t="n">
+        <v>11</v>
+      </c>
+      <c r="X197" t="inlineStr">
+        <is>
+          <t>ADC BOADILLA vs GRUPO EGIDO PINTOBASKET</t>
+        </is>
+      </c>
+    </row>
+    <row r="198">
+      <c r="A198" t="n">
+        <v>2487650</v>
+      </c>
+      <c r="B198" t="inlineStr">
+        <is>
+          <t>ADC BOADILLA</t>
+        </is>
+      </c>
+      <c r="C198" t="inlineStr">
+        <is>
+          <t>A. GOMEZ SERRANO | A. OLMEDO VELASCO | E. BOADA MONTESDEOCA | I. BLANCO-ARGIBAY GONZALEZ | P. DOMINGUEZ LORENZO</t>
+        </is>
+      </c>
+      <c r="D198" t="n">
+        <v>5</v>
+      </c>
+      <c r="E198" t="n">
+        <v>39</v>
+      </c>
+      <c r="F198" t="n">
+        <v>0.65</v>
+      </c>
+      <c r="G198" t="n">
+        <v>0</v>
+      </c>
+      <c r="H198" t="n">
+        <v>2</v>
+      </c>
+      <c r="I198" t="n">
+        <v>1</v>
+      </c>
+      <c r="J198" t="n">
+        <v>1</v>
+      </c>
+      <c r="K198" t="n">
+        <v>0</v>
+      </c>
+      <c r="L198" t="n">
+        <v>200</v>
+      </c>
+      <c r="M198" t="n">
+        <v>-200</v>
+      </c>
+      <c r="N198" t="n">
+        <v>0</v>
+      </c>
+      <c r="O198" t="n">
+        <v>0</v>
+      </c>
+      <c r="P198" t="n">
+        <v>1</v>
+      </c>
+      <c r="Q198" t="n">
+        <v>0</v>
+      </c>
+      <c r="R198" t="n">
+        <v>1</v>
+      </c>
+      <c r="S198" t="n">
+        <v>0</v>
+      </c>
+      <c r="T198" t="n">
+        <v>0</v>
+      </c>
+      <c r="U198" t="n">
+        <v>0</v>
+      </c>
+      <c r="V198" t="inlineStr">
+        <is>
+          <t>Liga Regular "B-B"</t>
+        </is>
+      </c>
+      <c r="W198" t="n">
+        <v>11</v>
+      </c>
+      <c r="X198" t="inlineStr">
+        <is>
+          <t>ADC BOADILLA vs GRUPO EGIDO PINTOBASKET</t>
+        </is>
+      </c>
+    </row>
+    <row r="199">
+      <c r="A199" t="n">
+        <v>2487650</v>
+      </c>
+      <c r="B199" t="inlineStr">
+        <is>
+          <t>ADC BOADILLA</t>
+        </is>
+      </c>
+      <c r="C199" t="inlineStr">
+        <is>
+          <t>A. GOMEZ SERRANO | A. OLMEDO VELASCO | I. BLANCO-ARGIBAY GONZALEZ | I. FINI | P. DOMINGUEZ LORENZO</t>
+        </is>
+      </c>
+      <c r="D199" t="n">
+        <v>5</v>
+      </c>
+      <c r="E199" t="n">
+        <v>20</v>
+      </c>
+      <c r="F199" t="n">
+        <v>0.33</v>
+      </c>
+      <c r="G199" t="n">
+        <v>0</v>
+      </c>
+      <c r="H199" t="n">
+        <v>3</v>
+      </c>
+      <c r="I199" t="n">
+        <v>0</v>
+      </c>
+      <c r="J199" t="n">
+        <v>0.88</v>
+      </c>
+      <c r="K199" t="inlineStr"/>
+      <c r="L199" t="n">
+        <v>340.91</v>
+      </c>
+      <c r="M199" t="inlineStr"/>
+      <c r="N199" t="n">
+        <v>0</v>
+      </c>
+      <c r="O199" t="n">
+        <v>0</v>
+      </c>
+      <c r="P199" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q199" t="n">
+        <v>0</v>
+      </c>
+      <c r="R199" t="n">
+        <v>3</v>
+      </c>
+      <c r="S199" t="n">
+        <v>2</v>
+      </c>
+      <c r="T199" t="n">
+        <v>0</v>
+      </c>
+      <c r="U199" t="n">
+        <v>3</v>
+      </c>
+      <c r="V199" t="inlineStr">
+        <is>
+          <t>Liga Regular "B-B"</t>
+        </is>
+      </c>
+      <c r="W199" t="n">
+        <v>11</v>
+      </c>
+      <c r="X199" t="inlineStr">
+        <is>
+          <t>ADC BOADILLA vs GRUPO EGIDO PINTOBASKET</t>
+        </is>
+      </c>
+    </row>
+    <row r="200">
+      <c r="A200" t="n">
+        <v>2487650</v>
+      </c>
+      <c r="B200" t="inlineStr">
+        <is>
+          <t>ADC BOADILLA</t>
+        </is>
+      </c>
+      <c r="C200" t="inlineStr">
+        <is>
+          <t>A. GOMEZ SERRANO | I. BLANCO-ARGIBAY GONZALEZ | I. FINI | M. SANCHEZ SANCHEZ | P. DOMINGUEZ LORENZO</t>
+        </is>
+      </c>
+      <c r="D200" t="n">
+        <v>5</v>
+      </c>
+      <c r="E200" t="n">
+        <v>14</v>
+      </c>
+      <c r="F200" t="n">
+        <v>0.23</v>
+      </c>
+      <c r="G200" t="n">
+        <v>3</v>
+      </c>
+      <c r="H200" t="n">
+        <v>0</v>
+      </c>
+      <c r="I200" t="n">
+        <v>1</v>
+      </c>
+      <c r="J200" t="n">
+        <v>0</v>
+      </c>
+      <c r="K200" t="n">
+        <v>300</v>
+      </c>
+      <c r="L200" t="inlineStr"/>
+      <c r="M200" t="inlineStr"/>
+      <c r="N200" t="n">
+        <v>1</v>
+      </c>
+      <c r="O200" t="n">
+        <v>0</v>
+      </c>
+      <c r="P200" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q200" t="n">
+        <v>0</v>
+      </c>
+      <c r="R200" t="n">
+        <v>0</v>
+      </c>
+      <c r="S200" t="n">
+        <v>0</v>
+      </c>
+      <c r="T200" t="n">
+        <v>0</v>
+      </c>
+      <c r="U200" t="n">
+        <v>0</v>
+      </c>
+      <c r="V200" t="inlineStr">
+        <is>
+          <t>Liga Regular "B-B"</t>
+        </is>
+      </c>
+      <c r="W200" t="n">
+        <v>11</v>
+      </c>
+      <c r="X200" t="inlineStr">
+        <is>
+          <t>ADC BOADILLA vs GRUPO EGIDO PINTOBASKET</t>
+        </is>
+      </c>
+    </row>
+    <row r="201">
+      <c r="A201" t="n">
+        <v>2487650</v>
+      </c>
+      <c r="B201" t="inlineStr">
+        <is>
+          <t>GRUPO EGIDO PINTOBASKET</t>
+        </is>
+      </c>
+      <c r="C201" t="inlineStr">
+        <is>
+          <t>C. BARROS CONDES | D. TOLOSA OROPESA | J. AYALA AYLLÓN | L. BERMEJO ALCALDE | M. ALARCON ORTIZ</t>
+        </is>
+      </c>
+      <c r="D201" t="n">
+        <v>5</v>
+      </c>
+      <c r="E201" t="n">
+        <v>812</v>
+      </c>
+      <c r="F201" t="n">
+        <v>13.53</v>
+      </c>
+      <c r="G201" t="n">
+        <v>21</v>
+      </c>
+      <c r="H201" t="n">
+        <v>20</v>
+      </c>
+      <c r="I201" t="n">
+        <v>24.28</v>
+      </c>
+      <c r="J201" t="n">
+        <v>18.96</v>
+      </c>
+      <c r="K201" t="n">
+        <v>86.48999999999999</v>
+      </c>
+      <c r="L201" t="n">
+        <v>105.49</v>
+      </c>
+      <c r="M201" t="n">
+        <v>-18.99</v>
+      </c>
+      <c r="N201" t="n">
+        <v>23</v>
+      </c>
+      <c r="O201" t="n">
+        <v>12</v>
+      </c>
+      <c r="P201" t="n">
+        <v>6</v>
+      </c>
+      <c r="Q201" t="n">
+        <v>10</v>
+      </c>
+      <c r="R201" t="n">
+        <v>15</v>
+      </c>
+      <c r="S201" t="n">
+        <v>9</v>
+      </c>
+      <c r="T201" t="n">
+        <v>7</v>
+      </c>
+      <c r="U201" t="n">
+        <v>7</v>
+      </c>
+      <c r="V201" t="inlineStr">
+        <is>
+          <t>Liga Regular "B-B"</t>
+        </is>
+      </c>
+      <c r="W201" t="n">
+        <v>11</v>
+      </c>
+      <c r="X201" t="inlineStr">
+        <is>
+          <t>ADC BOADILLA vs GRUPO EGIDO PINTOBASKET</t>
+        </is>
+      </c>
+    </row>
+    <row r="202">
+      <c r="A202" t="n">
+        <v>2487650</v>
+      </c>
+      <c r="B202" t="inlineStr">
+        <is>
+          <t>GRUPO EGIDO PINTOBASKET</t>
+        </is>
+      </c>
+      <c r="C202" t="inlineStr">
+        <is>
+          <t>C. BARROS CONDES | D. TOLOSA OROPESA | L. BERMEJO ALCALDE | M. ALARCON ORTIZ | M. SANZ CÁMARA</t>
+        </is>
+      </c>
+      <c r="D202" t="n">
+        <v>5</v>
+      </c>
+      <c r="E202" t="n">
+        <v>48</v>
+      </c>
+      <c r="F202" t="n">
+        <v>0.8</v>
+      </c>
+      <c r="G202" t="n">
+        <v>0</v>
+      </c>
+      <c r="H202" t="n">
+        <v>3</v>
+      </c>
+      <c r="I202" t="n">
+        <v>0</v>
+      </c>
+      <c r="J202" t="n">
+        <v>2</v>
+      </c>
+      <c r="K202" t="inlineStr"/>
+      <c r="L202" t="n">
+        <v>150</v>
+      </c>
+      <c r="M202" t="inlineStr"/>
+      <c r="N202" t="n">
+        <v>0</v>
+      </c>
+      <c r="O202" t="n">
+        <v>0</v>
+      </c>
+      <c r="P202" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q202" t="n">
+        <v>0</v>
+      </c>
+      <c r="R202" t="n">
+        <v>2</v>
+      </c>
+      <c r="S202" t="n">
+        <v>0</v>
+      </c>
+      <c r="T202" t="n">
+        <v>0</v>
+      </c>
+      <c r="U202" t="n">
+        <v>0</v>
+      </c>
+      <c r="V202" t="inlineStr">
+        <is>
+          <t>Liga Regular "B-B"</t>
+        </is>
+      </c>
+      <c r="W202" t="n">
+        <v>11</v>
+      </c>
+      <c r="X202" t="inlineStr">
+        <is>
+          <t>ADC BOADILLA vs GRUPO EGIDO PINTOBASKET</t>
+        </is>
+      </c>
+    </row>
+    <row r="203">
+      <c r="A203" t="n">
+        <v>2487660</v>
+      </c>
+      <c r="B203" t="inlineStr">
+        <is>
+          <t>BALONCESTO TELDE</t>
+        </is>
+      </c>
+      <c r="C203" t="inlineStr">
+        <is>
+          <t>A. FERNÁNDEZ GÓMEZ | A. REDONDO ALVAREZ DE SOTOMAYOR | D. VAZQUEZ JEREZ | I. MENCARA JIMENEZ | P. SÁNCHEZ GUTIERREZ</t>
+        </is>
+      </c>
+      <c r="D203" t="n">
+        <v>5</v>
+      </c>
+      <c r="E203" t="n">
+        <v>87</v>
+      </c>
+      <c r="F203" t="n">
+        <v>1.45</v>
+      </c>
+      <c r="G203" t="n">
+        <v>0</v>
+      </c>
+      <c r="H203" t="n">
+        <v>5</v>
+      </c>
+      <c r="I203" t="n">
+        <v>1.88</v>
+      </c>
+      <c r="J203" t="n">
+        <v>1</v>
+      </c>
+      <c r="K203" t="n">
+        <v>0</v>
+      </c>
+      <c r="L203" t="n">
+        <v>500</v>
+      </c>
+      <c r="M203" t="n">
+        <v>-500</v>
+      </c>
+      <c r="N203" t="n">
+        <v>1</v>
+      </c>
+      <c r="O203" t="n">
+        <v>2</v>
+      </c>
+      <c r="P203" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q203" t="n">
+        <v>0</v>
+      </c>
+      <c r="R203" t="n">
+        <v>2</v>
+      </c>
+      <c r="S203" t="n">
+        <v>0</v>
+      </c>
+      <c r="T203" t="n">
+        <v>0</v>
+      </c>
+      <c r="U203" t="n">
+        <v>1</v>
+      </c>
+      <c r="V203" t="inlineStr">
+        <is>
+          <t>Liga Regular "B-B"</t>
+        </is>
+      </c>
+      <c r="W203" t="n">
+        <v>12</v>
+      </c>
+      <c r="X203" t="inlineStr">
+        <is>
+          <t>BALONCESTO TELDE vs EB FELIPE ANTÓN</t>
+        </is>
+      </c>
+    </row>
+    <row r="204">
+      <c r="A204" t="n">
+        <v>2487660</v>
+      </c>
+      <c r="B204" t="inlineStr">
+        <is>
+          <t>BALONCESTO TELDE</t>
+        </is>
+      </c>
+      <c r="C204" t="inlineStr">
+        <is>
+          <t>A. MARTIN GONZALEZ | A. REDONDO ALVAREZ DE SOTOMAYOR | D. VAZQUEZ JEREZ | I. MENCARA JIMENEZ | P. SÁNCHEZ GUTIERREZ</t>
+        </is>
+      </c>
+      <c r="D204" t="n">
+        <v>5</v>
+      </c>
+      <c r="E204" t="n">
+        <v>45</v>
+      </c>
+      <c r="F204" t="n">
+        <v>0.75</v>
+      </c>
+      <c r="G204" t="n">
+        <v>0</v>
+      </c>
+      <c r="H204" t="n">
+        <v>0</v>
+      </c>
+      <c r="I204" t="n">
+        <v>1</v>
+      </c>
+      <c r="J204" t="n">
+        <v>0</v>
+      </c>
+      <c r="K204" t="n">
+        <v>0</v>
+      </c>
+      <c r="L204" t="inlineStr"/>
+      <c r="M204" t="inlineStr"/>
+      <c r="N204" t="n">
+        <v>1</v>
+      </c>
+      <c r="O204" t="n">
+        <v>0</v>
+      </c>
+      <c r="P204" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q204" t="n">
+        <v>0</v>
+      </c>
+      <c r="R204" t="n">
+        <v>1</v>
+      </c>
+      <c r="S204" t="n">
+        <v>0</v>
+      </c>
+      <c r="T204" t="n">
+        <v>0</v>
+      </c>
+      <c r="U204" t="n">
+        <v>1</v>
+      </c>
+      <c r="V204" t="inlineStr">
+        <is>
+          <t>Liga Regular "B-B"</t>
+        </is>
+      </c>
+      <c r="W204" t="n">
+        <v>12</v>
+      </c>
+      <c r="X204" t="inlineStr">
+        <is>
+          <t>BALONCESTO TELDE vs EB FELIPE ANTÓN</t>
+        </is>
+      </c>
+    </row>
+    <row r="205">
+      <c r="A205" t="n">
+        <v>2487660</v>
+      </c>
+      <c r="B205" t="inlineStr">
+        <is>
+          <t>BALONCESTO TELDE</t>
+        </is>
+      </c>
+      <c r="C205" t="inlineStr">
+        <is>
+          <t>A. FERNÁNDEZ GÓMEZ | A. REDONDO ALVAREZ DE SOTOMAYOR | D. VAZQUEZ JEREZ | G. ARTILES ROMERO | P. SÁNCHEZ GUTIERREZ</t>
+        </is>
+      </c>
+      <c r="D205" t="n">
+        <v>5</v>
+      </c>
+      <c r="E205" t="n">
+        <v>32</v>
+      </c>
+      <c r="F205" t="n">
+        <v>0.53</v>
+      </c>
+      <c r="G205" t="n">
+        <v>4</v>
+      </c>
+      <c r="H205" t="n">
+        <v>2</v>
+      </c>
+      <c r="I205" t="n">
+        <v>1.88</v>
+      </c>
+      <c r="J205" t="n">
+        <v>1</v>
+      </c>
+      <c r="K205" t="n">
+        <v>212.77</v>
+      </c>
+      <c r="L205" t="n">
+        <v>200</v>
+      </c>
+      <c r="M205" t="n">
+        <v>12.77</v>
+      </c>
+      <c r="N205" t="n">
+        <v>1</v>
+      </c>
+      <c r="O205" t="n">
+        <v>2</v>
+      </c>
+      <c r="P205" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q205" t="n">
+        <v>0</v>
+      </c>
+      <c r="R205" t="n">
+        <v>1</v>
+      </c>
+      <c r="S205" t="n">
+        <v>0</v>
+      </c>
+      <c r="T205" t="n">
+        <v>0</v>
+      </c>
+      <c r="U205" t="n">
+        <v>0</v>
+      </c>
+      <c r="V205" t="inlineStr">
+        <is>
+          <t>Liga Regular "B-B"</t>
+        </is>
+      </c>
+      <c r="W205" t="n">
+        <v>12</v>
+      </c>
+      <c r="X205" t="inlineStr">
+        <is>
+          <t>BALONCESTO TELDE vs EB FELIPE ANTÓN</t>
+        </is>
+      </c>
+    </row>
+    <row r="206">
+      <c r="A206" t="n">
+        <v>2487660</v>
+      </c>
+      <c r="B206" t="inlineStr">
+        <is>
+          <t>BALONCESTO TELDE</t>
+        </is>
+      </c>
+      <c r="C206" t="inlineStr">
+        <is>
+          <t>A. FERNÁNDEZ GÓMEZ | A. MARTIN GONZALEZ | A. REDONDO ALVAREZ DE SOTOMAYOR | D. VAZQUEZ JEREZ | P. SÁNCHEZ GUTIERREZ</t>
+        </is>
+      </c>
+      <c r="D206" t="n">
+        <v>5</v>
+      </c>
+      <c r="E206" t="n">
+        <v>24</v>
+      </c>
+      <c r="F206" t="n">
+        <v>0.4</v>
+      </c>
+      <c r="G206" t="n">
+        <v>0</v>
+      </c>
+      <c r="H206" t="n">
+        <v>0</v>
+      </c>
+      <c r="I206" t="n">
+        <v>0</v>
+      </c>
+      <c r="J206" t="n">
+        <v>1</v>
+      </c>
+      <c r="K206" t="inlineStr"/>
+      <c r="L206" t="n">
+        <v>0</v>
+      </c>
+      <c r="M206" t="inlineStr"/>
+      <c r="N206" t="n">
+        <v>1</v>
+      </c>
+      <c r="O206" t="n">
+        <v>0</v>
+      </c>
+      <c r="P206" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q206" t="n">
+        <v>1</v>
+      </c>
+      <c r="R206" t="n">
+        <v>1</v>
+      </c>
+      <c r="S206" t="n">
+        <v>0</v>
+      </c>
+      <c r="T206" t="n">
+        <v>0</v>
+      </c>
+      <c r="U206" t="n">
+        <v>0</v>
+      </c>
+      <c r="V206" t="inlineStr">
+        <is>
+          <t>Liga Regular "B-B"</t>
+        </is>
+      </c>
+      <c r="W206" t="n">
+        <v>12</v>
+      </c>
+      <c r="X206" t="inlineStr">
+        <is>
+          <t>BALONCESTO TELDE vs EB FELIPE ANTÓN</t>
+        </is>
+      </c>
+    </row>
+    <row r="207">
+      <c r="A207" t="n">
+        <v>2487660</v>
+      </c>
+      <c r="B207" t="inlineStr">
+        <is>
+          <t>BALONCESTO TELDE</t>
+        </is>
+      </c>
+      <c r="C207" t="inlineStr">
+        <is>
+          <t>A. FERNÁNDEZ GÓMEZ | A. MARTIN GONZALEZ | D. VAZQUEZ JEREZ | I. MENCARA JIMENEZ | P. SÁNCHEZ GUTIERREZ</t>
+        </is>
+      </c>
+      <c r="D207" t="n">
+        <v>5</v>
+      </c>
+      <c r="E207" t="n">
+        <v>4</v>
+      </c>
+      <c r="F207" t="n">
+        <v>0.07000000000000001</v>
+      </c>
+      <c r="G207" t="n">
+        <v>0</v>
+      </c>
+      <c r="H207" t="n">
+        <v>0</v>
+      </c>
+      <c r="I207" t="n">
+        <v>0</v>
+      </c>
+      <c r="J207" t="n">
+        <v>0</v>
+      </c>
+      <c r="K207" t="inlineStr"/>
+      <c r="L207" t="inlineStr"/>
+      <c r="M207" t="inlineStr"/>
+      <c r="N207" t="n">
+        <v>0</v>
+      </c>
+      <c r="O207" t="n">
+        <v>0</v>
+      </c>
+      <c r="P207" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q207" t="n">
+        <v>0</v>
+      </c>
+      <c r="R207" t="n">
+        <v>0</v>
+      </c>
+      <c r="S207" t="n">
+        <v>0</v>
+      </c>
+      <c r="T207" t="n">
+        <v>0</v>
+      </c>
+      <c r="U207" t="n">
+        <v>0</v>
+      </c>
+      <c r="V207" t="inlineStr">
+        <is>
+          <t>Liga Regular "B-B"</t>
+        </is>
+      </c>
+      <c r="W207" t="n">
+        <v>12</v>
+      </c>
+      <c r="X207" t="inlineStr">
+        <is>
+          <t>BALONCESTO TELDE vs EB FELIPE ANTÓN</t>
+        </is>
+      </c>
+    </row>
+    <row r="208">
+      <c r="A208" t="n">
+        <v>2487660</v>
+      </c>
+      <c r="B208" t="inlineStr">
+        <is>
+          <t>BALONCESTO TELDE</t>
+        </is>
+      </c>
+      <c r="C208" t="inlineStr">
+        <is>
+          <t>A. FERNÁNDEZ GÓMEZ | A. MARTIN GONZALEZ | A. REDONDO ALVAREZ DE SOTOMAYOR | I. MENCARA JIMENEZ | P. SÁNCHEZ GUTIERREZ</t>
+        </is>
+      </c>
+      <c r="D208" t="n">
+        <v>5</v>
+      </c>
+      <c r="E208" t="n">
+        <v>2</v>
+      </c>
+      <c r="F208" t="n">
+        <v>0.03</v>
+      </c>
+      <c r="G208" t="n">
+        <v>0</v>
+      </c>
+      <c r="H208" t="n">
+        <v>2</v>
+      </c>
+      <c r="I208" t="n">
+        <v>0</v>
+      </c>
+      <c r="J208" t="n">
+        <v>1</v>
+      </c>
+      <c r="K208" t="inlineStr"/>
+      <c r="L208" t="n">
+        <v>200</v>
+      </c>
+      <c r="M208" t="inlineStr"/>
+      <c r="N208" t="n">
+        <v>0</v>
+      </c>
+      <c r="O208" t="n">
+        <v>0</v>
+      </c>
+      <c r="P208" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q208" t="n">
+        <v>0</v>
+      </c>
+      <c r="R208" t="n">
+        <v>1</v>
+      </c>
+      <c r="S208" t="n">
+        <v>0</v>
+      </c>
+      <c r="T208" t="n">
+        <v>0</v>
+      </c>
+      <c r="U208" t="n">
+        <v>0</v>
+      </c>
+      <c r="V208" t="inlineStr">
+        <is>
+          <t>Liga Regular "B-B"</t>
+        </is>
+      </c>
+      <c r="W208" t="n">
+        <v>12</v>
+      </c>
+      <c r="X208" t="inlineStr">
+        <is>
+          <t>BALONCESTO TELDE vs EB FELIPE ANTÓN</t>
+        </is>
+      </c>
+    </row>
+    <row r="209">
+      <c r="A209" t="n">
+        <v>2487660</v>
+      </c>
+      <c r="B209" t="inlineStr">
+        <is>
+          <t>EB FELIPE ANTÓN</t>
+        </is>
+      </c>
+      <c r="C209" t="inlineStr">
+        <is>
+          <t>J. GALLETTO LAMELA | K. RIVEROL DE LAS CASAS | M. NIMAGA | P. ARGÜELLES ELORZA | S. MANERO GUZMAN</t>
+        </is>
+      </c>
+      <c r="D209" t="n">
+        <v>5</v>
+      </c>
+      <c r="E209" t="n">
+        <v>143</v>
+      </c>
+      <c r="F209" t="n">
+        <v>2.38</v>
+      </c>
+      <c r="G209" t="n">
+        <v>7</v>
+      </c>
+      <c r="H209" t="n">
+        <v>4</v>
+      </c>
+      <c r="I209" t="n">
+        <v>3</v>
+      </c>
+      <c r="J209" t="n">
+        <v>3.76</v>
+      </c>
+      <c r="K209" t="n">
+        <v>233.33</v>
+      </c>
+      <c r="L209" t="n">
+        <v>106.38</v>
+      </c>
+      <c r="M209" t="n">
+        <v>126.95</v>
+      </c>
+      <c r="N209" t="n">
+        <v>4</v>
+      </c>
+      <c r="O209" t="n">
+        <v>0</v>
+      </c>
+      <c r="P209" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q209" t="n">
+        <v>1</v>
+      </c>
+      <c r="R209" t="n">
+        <v>3</v>
+      </c>
+      <c r="S209" t="n">
+        <v>4</v>
+      </c>
+      <c r="T209" t="n">
+        <v>0</v>
+      </c>
+      <c r="U209" t="n">
+        <v>1</v>
+      </c>
+      <c r="V209" t="inlineStr">
+        <is>
+          <t>Liga Regular "B-B"</t>
+        </is>
+      </c>
+      <c r="W209" t="n">
+        <v>12</v>
+      </c>
+      <c r="X209" t="inlineStr">
+        <is>
+          <t>BALONCESTO TELDE vs EB FELIPE ANTÓN</t>
+        </is>
+      </c>
+    </row>
+    <row r="210">
+      <c r="A210" t="n">
+        <v>2487660</v>
+      </c>
+      <c r="B210" t="inlineStr">
+        <is>
+          <t>EB FELIPE ANTÓN</t>
+        </is>
+      </c>
+      <c r="C210" t="inlineStr">
+        <is>
+          <t>E. DUQUE NEGRÍN | J. GALLETTO LAMELA | K. RIVEROL DE LAS CASAS | M. NIMAGA | S. MANERO GUZMAN</t>
+        </is>
+      </c>
+      <c r="D210" t="n">
+        <v>5</v>
+      </c>
+      <c r="E210" t="n">
+        <v>45</v>
+      </c>
+      <c r="F210" t="n">
+        <v>0.75</v>
+      </c>
+      <c r="G210" t="n">
+        <v>0</v>
+      </c>
+      <c r="H210" t="n">
+        <v>0</v>
+      </c>
+      <c r="I210" t="n">
+        <v>0</v>
+      </c>
+      <c r="J210" t="n">
+        <v>1</v>
+      </c>
+      <c r="K210" t="inlineStr"/>
+      <c r="L210" t="n">
+        <v>0</v>
+      </c>
+      <c r="M210" t="inlineStr"/>
+      <c r="N210" t="n">
+        <v>1</v>
+      </c>
+      <c r="O210" t="n">
+        <v>0</v>
+      </c>
+      <c r="P210" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q210" t="n">
+        <v>1</v>
+      </c>
+      <c r="R210" t="n">
+        <v>1</v>
+      </c>
+      <c r="S210" t="n">
+        <v>0</v>
+      </c>
+      <c r="T210" t="n">
+        <v>0</v>
+      </c>
+      <c r="U210" t="n">
+        <v>0</v>
+      </c>
+      <c r="V210" t="inlineStr">
+        <is>
+          <t>Liga Regular "B-B"</t>
+        </is>
+      </c>
+      <c r="W210" t="n">
+        <v>12</v>
+      </c>
+      <c r="X210" t="inlineStr">
+        <is>
+          <t>BALONCESTO TELDE vs EB FELIPE ANTÓN</t>
+        </is>
+      </c>
+    </row>
+    <row r="211">
+      <c r="A211" t="n">
+        <v>2487660</v>
+      </c>
+      <c r="B211" t="inlineStr">
+        <is>
+          <t>EB FELIPE ANTÓN</t>
+        </is>
+      </c>
+      <c r="C211" t="inlineStr">
+        <is>
+          <t>E. DUQUE NEGRÍN | J. GALLETTO LAMELA | K. RIVEROL DE LAS CASAS | P. ARGÜELLES ELORZA | S. MANERO GUZMAN</t>
+        </is>
+      </c>
+      <c r="D211" t="n">
+        <v>5</v>
+      </c>
+      <c r="E211" t="n">
+        <v>4</v>
+      </c>
+      <c r="F211" t="n">
+        <v>0.07000000000000001</v>
+      </c>
+      <c r="G211" t="n">
+        <v>0</v>
+      </c>
+      <c r="H211" t="n">
+        <v>0</v>
+      </c>
+      <c r="I211" t="n">
+        <v>0</v>
+      </c>
+      <c r="J211" t="n">
+        <v>0</v>
+      </c>
+      <c r="K211" t="inlineStr"/>
+      <c r="L211" t="inlineStr"/>
+      <c r="M211" t="inlineStr"/>
+      <c r="N211" t="n">
+        <v>0</v>
+      </c>
+      <c r="O211" t="n">
+        <v>0</v>
+      </c>
+      <c r="P211" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q211" t="n">
+        <v>0</v>
+      </c>
+      <c r="R211" t="n">
+        <v>0</v>
+      </c>
+      <c r="S211" t="n">
+        <v>0</v>
+      </c>
+      <c r="T211" t="n">
+        <v>0</v>
+      </c>
+      <c r="U211" t="n">
+        <v>0</v>
+      </c>
+      <c r="V211" t="inlineStr">
+        <is>
+          <t>Liga Regular "B-B"</t>
+        </is>
+      </c>
+      <c r="W211" t="n">
+        <v>12</v>
+      </c>
+      <c r="X211" t="inlineStr">
+        <is>
+          <t>BALONCESTO TELDE vs EB FELIPE ANTÓN</t>
+        </is>
+      </c>
+    </row>
+    <row r="212">
+      <c r="A212" t="n">
+        <v>2487660</v>
+      </c>
+      <c r="B212" t="inlineStr">
+        <is>
+          <t>EB FELIPE ANTÓN</t>
+        </is>
+      </c>
+      <c r="C212" t="inlineStr">
+        <is>
+          <t>A. SISTAC RODRIGUEZ | E. DUQUE NEGRÍN | J. GALLETTO LAMELA | P. ARGÜELLES ELORZA | S. MANERO GUZMAN</t>
+        </is>
+      </c>
+      <c r="D212" t="n">
+        <v>5</v>
+      </c>
+      <c r="E212" t="n">
+        <v>2</v>
+      </c>
+      <c r="F212" t="n">
+        <v>0.03</v>
+      </c>
+      <c r="G212" t="n">
+        <v>2</v>
+      </c>
+      <c r="H212" t="n">
+        <v>0</v>
+      </c>
+      <c r="I212" t="n">
+        <v>1</v>
+      </c>
+      <c r="J212" t="n">
+        <v>0</v>
+      </c>
+      <c r="K212" t="n">
+        <v>200</v>
+      </c>
+      <c r="L212" t="inlineStr"/>
+      <c r="M212" t="inlineStr"/>
+      <c r="N212" t="n">
+        <v>1</v>
+      </c>
+      <c r="O212" t="n">
+        <v>0</v>
+      </c>
+      <c r="P212" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q212" t="n">
+        <v>0</v>
+      </c>
+      <c r="R212" t="n">
+        <v>0</v>
+      </c>
+      <c r="S212" t="n">
+        <v>0</v>
+      </c>
+      <c r="T212" t="n">
+        <v>0</v>
+      </c>
+      <c r="U212" t="n">
+        <v>0</v>
+      </c>
+      <c r="V212" t="inlineStr">
+        <is>
+          <t>Liga Regular "B-B"</t>
+        </is>
+      </c>
+      <c r="W212" t="n">
+        <v>12</v>
+      </c>
+      <c r="X212" t="inlineStr">
+        <is>
+          <t>BALONCESTO TELDE vs EB FELIPE ANTÓN</t>
+        </is>
+      </c>
+    </row>
+    <row r="213">
+      <c r="A213" t="n">
+        <v>2487655</v>
+      </c>
+      <c r="B213" t="inlineStr">
+        <is>
+          <t>LUJISA GUADALAJARA BASKET</t>
+        </is>
+      </c>
+      <c r="C213" t="inlineStr">
+        <is>
+          <t>A. ARMSTRONG | B. OJEDA OCHOA | D. EBOLO OLU-ELIJAH | F. DIAZ ZARZUELA | L. VALERA VILLEGAS</t>
+        </is>
+      </c>
+      <c r="D213" t="n">
+        <v>5</v>
+      </c>
+      <c r="E213" t="n">
+        <v>114</v>
+      </c>
+      <c r="F213" t="n">
+        <v>1.9</v>
+      </c>
+      <c r="G213" t="n">
+        <v>0</v>
+      </c>
+      <c r="H213" t="n">
+        <v>2</v>
+      </c>
+      <c r="I213" t="n">
+        <v>2</v>
+      </c>
+      <c r="J213" t="n">
+        <v>1.76</v>
+      </c>
+      <c r="K213" t="n">
+        <v>0</v>
+      </c>
+      <c r="L213" t="n">
+        <v>113.64</v>
+      </c>
+      <c r="M213" t="n">
+        <v>-113.64</v>
+      </c>
+      <c r="N213" t="n">
+        <v>2</v>
+      </c>
+      <c r="O213" t="n">
+        <v>0</v>
+      </c>
+      <c r="P213" t="n">
+        <v>1</v>
+      </c>
+      <c r="Q213" t="n">
+        <v>1</v>
+      </c>
+      <c r="R213" t="n">
+        <v>2</v>
+      </c>
+      <c r="S213" t="n">
+        <v>4</v>
+      </c>
+      <c r="T213" t="n">
+        <v>0</v>
+      </c>
+      <c r="U213" t="n">
+        <v>2</v>
+      </c>
+      <c r="V213" t="inlineStr">
+        <is>
+          <t>Liga Regular "B-B"</t>
+        </is>
+      </c>
+      <c r="W213" t="n">
+        <v>12</v>
+      </c>
+      <c r="X213" t="inlineStr">
+        <is>
+          <t>UROS DE RIVAS vs LUJISA GUADALAJARA BASKET</t>
+        </is>
+      </c>
+    </row>
+    <row r="214">
+      <c r="A214" t="n">
+        <v>2487655</v>
+      </c>
+      <c r="B214" t="inlineStr">
+        <is>
+          <t>LUJISA GUADALAJARA BASKET</t>
+        </is>
+      </c>
+      <c r="C214" t="inlineStr">
+        <is>
+          <t>B. OJEDA OCHOA | D. EBOLO OLU-ELIJAH | E. CALVO SALVE | L. VALERA VILLEGAS | M. DIALLO</t>
+        </is>
+      </c>
+      <c r="D214" t="n">
+        <v>5</v>
+      </c>
+      <c r="E214" t="n">
+        <v>106</v>
+      </c>
+      <c r="F214" t="n">
+        <v>1.77</v>
+      </c>
+      <c r="G214" t="n">
+        <v>6</v>
+      </c>
+      <c r="H214" t="n">
+        <v>2</v>
+      </c>
+      <c r="I214" t="n">
+        <v>4</v>
+      </c>
+      <c r="J214" t="n">
+        <v>3</v>
+      </c>
+      <c r="K214" t="n">
+        <v>150</v>
+      </c>
+      <c r="L214" t="n">
+        <v>66.67</v>
+      </c>
+      <c r="M214" t="n">
+        <v>83.33</v>
+      </c>
+      <c r="N214" t="n">
+        <v>4</v>
+      </c>
+      <c r="O214" t="n">
+        <v>0</v>
+      </c>
+      <c r="P214" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q214" t="n">
+        <v>0</v>
+      </c>
+      <c r="R214" t="n">
+        <v>2</v>
+      </c>
+      <c r="S214" t="n">
+        <v>0</v>
+      </c>
+      <c r="T214" t="n">
+        <v>2</v>
+      </c>
+      <c r="U214" t="n">
+        <v>1</v>
+      </c>
+      <c r="V214" t="inlineStr">
+        <is>
+          <t>Liga Regular "B-B"</t>
+        </is>
+      </c>
+      <c r="W214" t="n">
+        <v>12</v>
+      </c>
+      <c r="X214" t="inlineStr">
+        <is>
+          <t>UROS DE RIVAS vs LUJISA GUADALAJARA BASKET</t>
+        </is>
+      </c>
+    </row>
+    <row r="215">
+      <c r="A215" t="n">
+        <v>2487655</v>
+      </c>
+      <c r="B215" t="inlineStr">
+        <is>
+          <t>LUJISA GUADALAJARA BASKET</t>
+        </is>
+      </c>
+      <c r="C215" t="inlineStr">
+        <is>
+          <t>A. ARMSTRONG | B. OJEDA OCHOA | D. EBOLO OLU-ELIJAH | L. VALERA VILLEGAS | M. DIALLO</t>
+        </is>
+      </c>
+      <c r="D215" t="n">
+        <v>5</v>
+      </c>
+      <c r="E215" t="n">
+        <v>53</v>
+      </c>
+      <c r="F215" t="n">
+        <v>0.88</v>
+      </c>
+      <c r="G215" t="n">
+        <v>0</v>
+      </c>
+      <c r="H215" t="n">
+        <v>2</v>
+      </c>
+      <c r="I215" t="n">
+        <v>2</v>
+      </c>
+      <c r="J215" t="n">
+        <v>1.88</v>
+      </c>
+      <c r="K215" t="n">
+        <v>0</v>
+      </c>
+      <c r="L215" t="n">
+        <v>106.38</v>
+      </c>
+      <c r="M215" t="n">
+        <v>-106.38</v>
+      </c>
+      <c r="N215" t="n">
+        <v>0</v>
+      </c>
+      <c r="O215" t="n">
+        <v>0</v>
+      </c>
+      <c r="P215" t="n">
+        <v>2</v>
+      </c>
+      <c r="Q215" t="n">
+        <v>0</v>
+      </c>
+      <c r="R215" t="n">
+        <v>2</v>
+      </c>
+      <c r="S215" t="n">
+        <v>2</v>
+      </c>
+      <c r="T215" t="n">
+        <v>0</v>
+      </c>
+      <c r="U215" t="n">
+        <v>1</v>
+      </c>
+      <c r="V215" t="inlineStr">
+        <is>
+          <t>Liga Regular "B-B"</t>
+        </is>
+      </c>
+      <c r="W215" t="n">
+        <v>12</v>
+      </c>
+      <c r="X215" t="inlineStr">
+        <is>
+          <t>UROS DE RIVAS vs LUJISA GUADALAJARA BASKET</t>
+        </is>
+      </c>
+    </row>
+    <row r="216">
+      <c r="A216" t="n">
+        <v>2487655</v>
+      </c>
+      <c r="B216" t="inlineStr">
+        <is>
+          <t>LUJISA GUADALAJARA BASKET</t>
+        </is>
+      </c>
+      <c r="C216" t="inlineStr">
+        <is>
+          <t>A. ARMSTRONG | B. OJEDA OCHOA | E. CALVO SALVE | F. DIAZ ZARZUELA | L. VALERA VILLEGAS</t>
+        </is>
+      </c>
+      <c r="D216" t="n">
+        <v>5</v>
+      </c>
+      <c r="E216" t="n">
+        <v>11</v>
+      </c>
+      <c r="F216" t="n">
+        <v>0.18</v>
+      </c>
+      <c r="G216" t="n">
+        <v>0</v>
+      </c>
+      <c r="H216" t="n">
+        <v>2</v>
+      </c>
+      <c r="I216" t="n">
+        <v>0.88</v>
+      </c>
+      <c r="J216" t="n">
+        <v>-0.12</v>
+      </c>
+      <c r="K216" t="n">
+        <v>0</v>
+      </c>
+      <c r="L216" t="inlineStr"/>
+      <c r="M216" t="inlineStr"/>
+      <c r="N216" t="n">
+        <v>0</v>
+      </c>
+      <c r="O216" t="n">
+        <v>2</v>
+      </c>
+      <c r="P216" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q216" t="n">
+        <v>0</v>
+      </c>
+      <c r="R216" t="n">
+        <v>0</v>
+      </c>
+      <c r="S216" t="n">
+        <v>2</v>
+      </c>
+      <c r="T216" t="n">
+        <v>0</v>
+      </c>
+      <c r="U216" t="n">
+        <v>1</v>
+      </c>
+      <c r="V216" t="inlineStr">
+        <is>
+          <t>Liga Regular "B-B"</t>
+        </is>
+      </c>
+      <c r="W216" t="n">
+        <v>12</v>
+      </c>
+      <c r="X216" t="inlineStr">
+        <is>
+          <t>UROS DE RIVAS vs LUJISA GUADALAJARA BASKET</t>
+        </is>
+      </c>
+    </row>
+    <row r="217">
+      <c r="A217" t="n">
+        <v>2487655</v>
+      </c>
+      <c r="B217" t="inlineStr">
+        <is>
+          <t>UROS DE RIVAS</t>
+        </is>
+      </c>
+      <c r="C217" t="inlineStr">
+        <is>
+          <t>A. BIERSACK LOPEZ | C. CRESPO MONTESINOS | D. MARINEZ FERNANDEZ-URRUTIA | O. HADI ADEGBITE | P. ESTEBANEZ GONZALEZ</t>
+        </is>
+      </c>
+      <c r="D217" t="n">
+        <v>5</v>
+      </c>
+      <c r="E217" t="n">
+        <v>106</v>
+      </c>
+      <c r="F217" t="n">
+        <v>1.77</v>
+      </c>
+      <c r="G217" t="n">
+        <v>2</v>
+      </c>
+      <c r="H217" t="n">
+        <v>6</v>
+      </c>
+      <c r="I217" t="n">
+        <v>3</v>
+      </c>
+      <c r="J217" t="n">
+        <v>4</v>
+      </c>
+      <c r="K217" t="n">
+        <v>66.67</v>
+      </c>
+      <c r="L217" t="n">
+        <v>150</v>
+      </c>
+      <c r="M217" t="n">
+        <v>-83.33</v>
+      </c>
+      <c r="N217" t="n">
+        <v>2</v>
+      </c>
+      <c r="O217" t="n">
+        <v>0</v>
+      </c>
+      <c r="P217" t="n">
+        <v>2</v>
+      </c>
+      <c r="Q217" t="n">
+        <v>1</v>
+      </c>
+      <c r="R217" t="n">
+        <v>4</v>
+      </c>
+      <c r="S217" t="n">
+        <v>0</v>
+      </c>
+      <c r="T217" t="n">
+        <v>0</v>
+      </c>
+      <c r="U217" t="n">
+        <v>0</v>
+      </c>
+      <c r="V217" t="inlineStr">
+        <is>
+          <t>Liga Regular "B-B"</t>
+        </is>
+      </c>
+      <c r="W217" t="n">
+        <v>12</v>
+      </c>
+      <c r="X217" t="inlineStr">
+        <is>
+          <t>UROS DE RIVAS vs LUJISA GUADALAJARA BASKET</t>
+        </is>
+      </c>
+    </row>
+    <row r="218">
+      <c r="A218" t="n">
+        <v>2487655</v>
+      </c>
+      <c r="B218" t="inlineStr">
+        <is>
+          <t>UROS DE RIVAS</t>
+        </is>
+      </c>
+      <c r="C218" t="inlineStr">
+        <is>
+          <t>A. BIERSACK LOPEZ | A. GARCIA QUILEZ CUERVAS | C. CRESPO MONTESINOS | D. MARINEZ FERNANDEZ-URRUTIA | P. ESTEBANEZ GONZALEZ</t>
+        </is>
+      </c>
+      <c r="D218" t="n">
+        <v>5</v>
+      </c>
+      <c r="E218" t="n">
+        <v>80</v>
+      </c>
+      <c r="F218" t="n">
+        <v>1.33</v>
+      </c>
+      <c r="G218" t="n">
+        <v>1</v>
+      </c>
+      <c r="H218" t="n">
+        <v>0</v>
+      </c>
+      <c r="I218" t="n">
+        <v>-0.12</v>
+      </c>
+      <c r="J218" t="n">
+        <v>1</v>
+      </c>
+      <c r="K218" t="inlineStr"/>
+      <c r="L218" t="n">
+        <v>0</v>
+      </c>
+      <c r="M218" t="inlineStr"/>
+      <c r="N218" t="n">
+        <v>1</v>
+      </c>
+      <c r="O218" t="n">
+        <v>2</v>
+      </c>
+      <c r="P218" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q218" t="n">
+        <v>2</v>
+      </c>
+      <c r="R218" t="n">
+        <v>2</v>
+      </c>
+      <c r="S218" t="n">
+        <v>0</v>
+      </c>
+      <c r="T218" t="n">
+        <v>0</v>
+      </c>
+      <c r="U218" t="n">
+        <v>1</v>
+      </c>
+      <c r="V218" t="inlineStr">
+        <is>
+          <t>Liga Regular "B-B"</t>
+        </is>
+      </c>
+      <c r="W218" t="n">
+        <v>12</v>
+      </c>
+      <c r="X218" t="inlineStr">
+        <is>
+          <t>UROS DE RIVAS vs LUJISA GUADALAJARA BASKET</t>
+        </is>
+      </c>
+    </row>
+    <row r="219">
+      <c r="A219" t="n">
+        <v>2487655</v>
+      </c>
+      <c r="B219" t="inlineStr">
+        <is>
+          <t>UROS DE RIVAS</t>
+        </is>
+      </c>
+      <c r="C219" t="inlineStr">
+        <is>
+          <t>A. BIERSACK LOPEZ | C. CRESPO MONTESINOS | D. MARINEZ FERNANDEZ-URRUTIA | M. VILLAMANDOS TORRES | P. ESTEBANEZ GONZALEZ</t>
+        </is>
+      </c>
+      <c r="D219" t="n">
+        <v>5</v>
+      </c>
+      <c r="E219" t="n">
+        <v>53</v>
+      </c>
+      <c r="F219" t="n">
+        <v>0.88</v>
+      </c>
+      <c r="G219" t="n">
+        <v>2</v>
+      </c>
+      <c r="H219" t="n">
+        <v>0</v>
+      </c>
+      <c r="I219" t="n">
+        <v>1.88</v>
+      </c>
+      <c r="J219" t="n">
+        <v>2</v>
+      </c>
+      <c r="K219" t="n">
+        <v>106.38</v>
+      </c>
+      <c r="L219" t="n">
+        <v>0</v>
+      </c>
+      <c r="M219" t="n">
+        <v>106.38</v>
+      </c>
+      <c r="N219" t="n">
+        <v>2</v>
+      </c>
+      <c r="O219" t="n">
+        <v>2</v>
+      </c>
+      <c r="P219" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q219" t="n">
+        <v>1</v>
+      </c>
+      <c r="R219" t="n">
+        <v>0</v>
+      </c>
+      <c r="S219" t="n">
+        <v>0</v>
+      </c>
+      <c r="T219" t="n">
+        <v>2</v>
+      </c>
+      <c r="U219" t="n">
+        <v>0</v>
+      </c>
+      <c r="V219" t="inlineStr">
+        <is>
+          <t>Liga Regular "B-B"</t>
+        </is>
+      </c>
+      <c r="W219" t="n">
+        <v>12</v>
+      </c>
+      <c r="X219" t="inlineStr">
+        <is>
+          <t>UROS DE RIVAS vs LUJISA GUADALAJARA BASKET</t>
+        </is>
+      </c>
+    </row>
+    <row r="220">
+      <c r="A220" t="n">
+        <v>2487655</v>
+      </c>
+      <c r="B220" t="inlineStr">
+        <is>
+          <t>UROS DE RIVAS</t>
+        </is>
+      </c>
+      <c r="C220" t="inlineStr">
+        <is>
+          <t>A. BIERSACK LOPEZ | A. GARCIA QUILEZ CUERVAS | C. CRESPO MONTESINOS | M. VILLAMANDOS TORRES | P. ESTEBANEZ GONZALEZ</t>
+        </is>
+      </c>
+      <c r="D220" t="n">
+        <v>5</v>
+      </c>
+      <c r="E220" t="n">
+        <v>45</v>
+      </c>
+      <c r="F220" t="n">
+        <v>0.75</v>
+      </c>
+      <c r="G220" t="n">
+        <v>3</v>
+      </c>
+      <c r="H220" t="n">
+        <v>0</v>
+      </c>
+      <c r="I220" t="n">
+        <v>1.76</v>
+      </c>
+      <c r="J220" t="n">
+        <v>1.88</v>
+      </c>
+      <c r="K220" t="n">
+        <v>170.45</v>
+      </c>
+      <c r="L220" t="n">
+        <v>0</v>
+      </c>
+      <c r="M220" t="n">
+        <v>170.45</v>
+      </c>
+      <c r="N220" t="n">
+        <v>1</v>
+      </c>
+      <c r="O220" t="n">
+        <v>4</v>
+      </c>
+      <c r="P220" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q220" t="n">
+        <v>1</v>
+      </c>
+      <c r="R220" t="n">
+        <v>0</v>
+      </c>
+      <c r="S220" t="n">
+        <v>2</v>
+      </c>
+      <c r="T220" t="n">
+        <v>1</v>
+      </c>
+      <c r="U220" t="n">
+        <v>0</v>
+      </c>
+      <c r="V220" t="inlineStr">
+        <is>
+          <t>Liga Regular "B-B"</t>
+        </is>
+      </c>
+      <c r="W220" t="n">
+        <v>12</v>
+      </c>
+      <c r="X220" t="inlineStr">
+        <is>
+          <t>UROS DE RIVAS vs LUJISA GUADALAJARA BASKET</t>
+        </is>
+      </c>
+    </row>
+    <row r="221">
+      <c r="A221" t="n">
+        <v>2487657</v>
+      </c>
+      <c r="B221" t="inlineStr">
+        <is>
+          <t>GRUPO EGIDO PINTOBASKET</t>
+        </is>
+      </c>
+      <c r="C221" t="inlineStr">
+        <is>
+          <t>C. BARROS CONDES | M. ALARCON ORTIZ | M. BATLLE BERNARDO | M. SANZ CÁMARA | S. RODRIGUEZ GREGORIO</t>
+        </is>
+      </c>
+      <c r="D221" t="n">
+        <v>5</v>
+      </c>
+      <c r="E221" t="n">
+        <v>147</v>
+      </c>
+      <c r="F221" t="n">
+        <v>2.45</v>
+      </c>
+      <c r="G221" t="n">
+        <v>0</v>
+      </c>
+      <c r="H221" t="n">
+        <v>5</v>
+      </c>
+      <c r="I221" t="n">
+        <v>6</v>
+      </c>
+      <c r="J221" t="n">
+        <v>5</v>
+      </c>
+      <c r="K221" t="n">
+        <v>0</v>
+      </c>
+      <c r="L221" t="n">
+        <v>100</v>
+      </c>
+      <c r="M221" t="n">
+        <v>-100</v>
+      </c>
+      <c r="N221" t="n">
+        <v>6</v>
+      </c>
+      <c r="O221" t="n">
+        <v>0</v>
+      </c>
+      <c r="P221" t="n">
+        <v>1</v>
+      </c>
+      <c r="Q221" t="n">
+        <v>1</v>
+      </c>
+      <c r="R221" t="n">
+        <v>3</v>
+      </c>
+      <c r="S221" t="n">
+        <v>0</v>
+      </c>
+      <c r="T221" t="n">
+        <v>2</v>
+      </c>
+      <c r="U221" t="n">
+        <v>0</v>
+      </c>
+      <c r="V221" t="inlineStr">
+        <is>
+          <t>Liga Regular "B-B"</t>
+        </is>
+      </c>
+      <c r="W221" t="n">
+        <v>12</v>
+      </c>
+      <c r="X221" t="inlineStr">
+        <is>
+          <t>GRUPO EGIDO PINTOBASKET vs RECUCYM BAZU</t>
+        </is>
+      </c>
+    </row>
+    <row r="222">
+      <c r="A222" t="n">
+        <v>2487657</v>
+      </c>
+      <c r="B222" t="inlineStr">
+        <is>
+          <t>GRUPO EGIDO PINTOBASKET</t>
+        </is>
+      </c>
+      <c r="C222" t="inlineStr">
+        <is>
+          <t>J. AYALA AYLLÓN | L. BERMEJO ALCALDE | M. ALARCON ORTIZ | M. BATLLE BERNARDO | S. RODRIGUEZ GREGORIO</t>
+        </is>
+      </c>
+      <c r="D222" t="n">
+        <v>5</v>
+      </c>
+      <c r="E222" t="n">
+        <v>70</v>
+      </c>
+      <c r="F222" t="n">
+        <v>1.17</v>
+      </c>
+      <c r="G222" t="n">
+        <v>0</v>
+      </c>
+      <c r="H222" t="n">
+        <v>3</v>
+      </c>
+      <c r="I222" t="n">
+        <v>3</v>
+      </c>
+      <c r="J222" t="n">
+        <v>2.88</v>
+      </c>
+      <c r="K222" t="n">
+        <v>0</v>
+      </c>
+      <c r="L222" t="n">
+        <v>104.17</v>
+      </c>
+      <c r="M222" t="n">
+        <v>-104.17</v>
+      </c>
+      <c r="N222" t="n">
+        <v>3</v>
+      </c>
+      <c r="O222" t="n">
+        <v>0</v>
+      </c>
+      <c r="P222" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q222" t="n">
+        <v>0</v>
+      </c>
+      <c r="R222" t="n">
+        <v>1</v>
+      </c>
+      <c r="S222" t="n">
+        <v>2</v>
+      </c>
+      <c r="T222" t="n">
+        <v>2</v>
+      </c>
+      <c r="U222" t="n">
+        <v>1</v>
+      </c>
+      <c r="V222" t="inlineStr">
+        <is>
+          <t>Liga Regular "B-B"</t>
+        </is>
+      </c>
+      <c r="W222" t="n">
+        <v>12</v>
+      </c>
+      <c r="X222" t="inlineStr">
+        <is>
+          <t>GRUPO EGIDO PINTOBASKET vs RECUCYM BAZU</t>
+        </is>
+      </c>
+    </row>
+    <row r="223">
+      <c r="A223" t="n">
+        <v>2487657</v>
+      </c>
+      <c r="B223" t="inlineStr">
+        <is>
+          <t>GRUPO EGIDO PINTOBASKET</t>
+        </is>
+      </c>
+      <c r="C223" t="inlineStr">
+        <is>
+          <t>C. BARROS CONDES | J. AYALA AYLLÓN | M. ALARCON ORTIZ | M. BATLLE BERNARDO | S. RODRIGUEZ GREGORIO</t>
+        </is>
+      </c>
+      <c r="D223" t="n">
+        <v>5</v>
+      </c>
+      <c r="E223" t="n">
+        <v>64</v>
+      </c>
+      <c r="F223" t="n">
+        <v>1.07</v>
+      </c>
+      <c r="G223" t="n">
+        <v>1</v>
+      </c>
+      <c r="H223" t="n">
+        <v>1</v>
+      </c>
+      <c r="I223" t="n">
+        <v>2.88</v>
+      </c>
+      <c r="J223" t="n">
+        <v>1.88</v>
+      </c>
+      <c r="K223" t="n">
+        <v>34.72</v>
+      </c>
+      <c r="L223" t="n">
+        <v>53.19</v>
+      </c>
+      <c r="M223" t="n">
+        <v>-18.47</v>
+      </c>
+      <c r="N223" t="n">
+        <v>1</v>
+      </c>
+      <c r="O223" t="n">
+        <v>2</v>
+      </c>
+      <c r="P223" t="n">
+        <v>1</v>
+      </c>
+      <c r="Q223" t="n">
+        <v>0</v>
+      </c>
+      <c r="R223" t="n">
+        <v>2</v>
+      </c>
+      <c r="S223" t="n">
+        <v>2</v>
+      </c>
+      <c r="T223" t="n">
+        <v>0</v>
+      </c>
+      <c r="U223" t="n">
+        <v>1</v>
+      </c>
+      <c r="V223" t="inlineStr">
+        <is>
+          <t>Liga Regular "B-B"</t>
+        </is>
+      </c>
+      <c r="W223" t="n">
+        <v>12</v>
+      </c>
+      <c r="X223" t="inlineStr">
+        <is>
+          <t>GRUPO EGIDO PINTOBASKET vs RECUCYM BAZU</t>
+        </is>
+      </c>
+    </row>
+    <row r="224">
+      <c r="A224" t="n">
+        <v>2487657</v>
+      </c>
+      <c r="B224" t="inlineStr">
+        <is>
+          <t>GRUPO EGIDO PINTOBASKET</t>
+        </is>
+      </c>
+      <c r="C224" t="inlineStr">
+        <is>
+          <t>C. BARROS CONDES | D. TOLOSA OROPESA | J. AYALA AYLLÓN | M. SANZ CÁMARA | S. RODRIGUEZ GREGORIO</t>
+        </is>
+      </c>
+      <c r="D224" t="n">
+        <v>5</v>
+      </c>
+      <c r="E224" t="n">
+        <v>58</v>
+      </c>
+      <c r="F224" t="n">
+        <v>0.97</v>
+      </c>
+      <c r="G224" t="n">
+        <v>3</v>
+      </c>
+      <c r="H224" t="n">
+        <v>3</v>
+      </c>
+      <c r="I224" t="n">
+        <v>2</v>
+      </c>
+      <c r="J224" t="n">
+        <v>2.88</v>
+      </c>
+      <c r="K224" t="n">
+        <v>150</v>
+      </c>
+      <c r="L224" t="n">
+        <v>104.17</v>
+      </c>
+      <c r="M224" t="n">
+        <v>45.83</v>
+      </c>
+      <c r="N224" t="n">
+        <v>1</v>
+      </c>
+      <c r="O224" t="n">
+        <v>0</v>
+      </c>
+      <c r="P224" t="n">
+        <v>1</v>
+      </c>
+      <c r="Q224" t="n">
+        <v>0</v>
+      </c>
+      <c r="R224" t="n">
+        <v>3</v>
+      </c>
+      <c r="S224" t="n">
+        <v>2</v>
+      </c>
+      <c r="T224" t="n">
+        <v>0</v>
+      </c>
+      <c r="U224" t="n">
+        <v>1</v>
+      </c>
+      <c r="V224" t="inlineStr">
+        <is>
+          <t>Liga Regular "B-B"</t>
+        </is>
+      </c>
+      <c r="W224" t="n">
+        <v>12</v>
+      </c>
+      <c r="X224" t="inlineStr">
+        <is>
+          <t>GRUPO EGIDO PINTOBASKET vs RECUCYM BAZU</t>
+        </is>
+      </c>
+    </row>
+    <row r="225">
+      <c r="A225" t="n">
+        <v>2487657</v>
+      </c>
+      <c r="B225" t="inlineStr">
+        <is>
+          <t>GRUPO EGIDO PINTOBASKET</t>
+        </is>
+      </c>
+      <c r="C225" t="inlineStr">
+        <is>
+          <t>C. BARROS CONDES | D. TOLOSA OROPESA | M. DEL VALLE REGALADO | M. SANZ CÁMARA | S. RODRIGUEZ GREGORIO</t>
+        </is>
+      </c>
+      <c r="D225" t="n">
+        <v>5</v>
+      </c>
+      <c r="E225" t="n">
+        <v>37</v>
+      </c>
+      <c r="F225" t="n">
+        <v>0.62</v>
+      </c>
+      <c r="G225" t="n">
+        <v>3</v>
+      </c>
+      <c r="H225" t="n">
+        <v>2</v>
+      </c>
+      <c r="I225" t="n">
+        <v>1</v>
+      </c>
+      <c r="J225" t="n">
+        <v>2</v>
+      </c>
+      <c r="K225" t="n">
+        <v>300</v>
+      </c>
+      <c r="L225" t="n">
+        <v>100</v>
+      </c>
+      <c r="M225" t="n">
+        <v>200</v>
+      </c>
+      <c r="N225" t="n">
+        <v>1</v>
+      </c>
+      <c r="O225" t="n">
+        <v>0</v>
+      </c>
+      <c r="P225" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q225" t="n">
+        <v>0</v>
+      </c>
+      <c r="R225" t="n">
+        <v>1</v>
+      </c>
+      <c r="S225" t="n">
+        <v>0</v>
+      </c>
+      <c r="T225" t="n">
+        <v>1</v>
+      </c>
+      <c r="U225" t="n">
+        <v>0</v>
+      </c>
+      <c r="V225" t="inlineStr">
+        <is>
+          <t>Liga Regular "B-B"</t>
+        </is>
+      </c>
+      <c r="W225" t="n">
+        <v>12</v>
+      </c>
+      <c r="X225" t="inlineStr">
+        <is>
+          <t>GRUPO EGIDO PINTOBASKET vs RECUCYM BAZU</t>
+        </is>
+      </c>
+    </row>
+    <row r="226">
+      <c r="A226" t="n">
+        <v>2487657</v>
+      </c>
+      <c r="B226" t="inlineStr">
+        <is>
+          <t>GRUPO EGIDO PINTOBASKET</t>
+        </is>
+      </c>
+      <c r="C226" t="inlineStr">
+        <is>
+          <t>D. TOLOSA OROPESA | J. AYALA AYLLÓN | L. BERMEJO ALCALDE | M. BATLLE BERNARDO | S. RODRIGUEZ GREGORIO</t>
+        </is>
+      </c>
+      <c r="D226" t="n">
+        <v>5</v>
+      </c>
+      <c r="E226" t="n">
+        <v>22</v>
+      </c>
+      <c r="F226" t="n">
+        <v>0.37</v>
+      </c>
+      <c r="G226" t="n">
+        <v>0</v>
+      </c>
+      <c r="H226" t="n">
+        <v>0</v>
+      </c>
+      <c r="I226" t="n">
+        <v>1</v>
+      </c>
+      <c r="J226" t="n">
+        <v>0</v>
+      </c>
+      <c r="K226" t="n">
+        <v>0</v>
+      </c>
+      <c r="L226" t="inlineStr"/>
+      <c r="M226" t="inlineStr"/>
+      <c r="N226" t="n">
+        <v>1</v>
+      </c>
+      <c r="O226" t="n">
+        <v>0</v>
+      </c>
+      <c r="P226" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q226" t="n">
+        <v>0</v>
+      </c>
+      <c r="R226" t="n">
+        <v>1</v>
+      </c>
+      <c r="S226" t="n">
+        <v>0</v>
+      </c>
+      <c r="T226" t="n">
+        <v>0</v>
+      </c>
+      <c r="U226" t="n">
+        <v>1</v>
+      </c>
+      <c r="V226" t="inlineStr">
+        <is>
+          <t>Liga Regular "B-B"</t>
+        </is>
+      </c>
+      <c r="W226" t="n">
+        <v>12</v>
+      </c>
+      <c r="X226" t="inlineStr">
+        <is>
+          <t>GRUPO EGIDO PINTOBASKET vs RECUCYM BAZU</t>
+        </is>
+      </c>
+    </row>
+    <row r="227">
+      <c r="A227" t="n">
+        <v>2487657</v>
+      </c>
+      <c r="B227" t="inlineStr">
+        <is>
+          <t>GRUPO EGIDO PINTOBASKET</t>
+        </is>
+      </c>
+      <c r="C227" t="inlineStr">
+        <is>
+          <t>C. BARROS CONDES | L. BERMEJO ALCALDE | M. ALARCON ORTIZ | M. DEL VALLE REGALADO | S. RODRIGUEZ GREGORIO</t>
+        </is>
+      </c>
+      <c r="D227" t="n">
+        <v>5</v>
+      </c>
+      <c r="E227" t="n">
+        <v>22</v>
+      </c>
+      <c r="F227" t="n">
+        <v>0.37</v>
+      </c>
+      <c r="G227" t="n">
+        <v>0</v>
+      </c>
+      <c r="H227" t="n">
+        <v>2</v>
+      </c>
+      <c r="I227" t="n">
+        <v>0</v>
+      </c>
+      <c r="J227" t="n">
+        <v>1</v>
+      </c>
+      <c r="K227" t="inlineStr"/>
+      <c r="L227" t="n">
+        <v>200</v>
+      </c>
+      <c r="M227" t="inlineStr"/>
+      <c r="N227" t="n">
+        <v>0</v>
+      </c>
+      <c r="O227" t="n">
+        <v>0</v>
+      </c>
+      <c r="P227" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q227" t="n">
+        <v>0</v>
+      </c>
+      <c r="R227" t="n">
+        <v>1</v>
+      </c>
+      <c r="S227" t="n">
+        <v>0</v>
+      </c>
+      <c r="T227" t="n">
+        <v>0</v>
+      </c>
+      <c r="U227" t="n">
+        <v>0</v>
+      </c>
+      <c r="V227" t="inlineStr">
+        <is>
+          <t>Liga Regular "B-B"</t>
+        </is>
+      </c>
+      <c r="W227" t="n">
+        <v>12</v>
+      </c>
+      <c r="X227" t="inlineStr">
+        <is>
+          <t>GRUPO EGIDO PINTOBASKET vs RECUCYM BAZU</t>
+        </is>
+      </c>
+    </row>
+    <row r="228">
+      <c r="A228" t="n">
+        <v>2487657</v>
+      </c>
+      <c r="B228" t="inlineStr">
+        <is>
+          <t>GRUPO EGIDO PINTOBASKET</t>
+        </is>
+      </c>
+      <c r="C228" t="inlineStr">
+        <is>
+          <t>D. TOLOSA OROPESA | L. BERMEJO ALCALDE | M. ALARCON ORTIZ | M. BATLLE BERNARDO | S. RODRIGUEZ GREGORIO</t>
+        </is>
+      </c>
+      <c r="D228" t="n">
+        <v>5</v>
+      </c>
+      <c r="E228" t="n">
+        <v>16</v>
+      </c>
+      <c r="F228" t="n">
+        <v>0.27</v>
+      </c>
+      <c r="G228" t="n">
+        <v>2</v>
+      </c>
+      <c r="H228" t="n">
+        <v>2</v>
+      </c>
+      <c r="I228" t="n">
+        <v>0.88</v>
+      </c>
+      <c r="J228" t="n">
+        <v>1</v>
+      </c>
+      <c r="K228" t="n">
+        <v>227.27</v>
+      </c>
+      <c r="L228" t="n">
+        <v>200</v>
+      </c>
+      <c r="M228" t="n">
+        <v>27.27</v>
+      </c>
+      <c r="N228" t="n">
+        <v>0</v>
+      </c>
+      <c r="O228" t="n">
+        <v>2</v>
+      </c>
+      <c r="P228" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q228" t="n">
+        <v>0</v>
+      </c>
+      <c r="R228" t="n">
+        <v>1</v>
+      </c>
+      <c r="S228" t="n">
+        <v>0</v>
+      </c>
+      <c r="T228" t="n">
+        <v>0</v>
+      </c>
+      <c r="U228" t="n">
+        <v>0</v>
+      </c>
+      <c r="V228" t="inlineStr">
+        <is>
+          <t>Liga Regular "B-B"</t>
+        </is>
+      </c>
+      <c r="W228" t="n">
+        <v>12</v>
+      </c>
+      <c r="X228" t="inlineStr">
+        <is>
+          <t>GRUPO EGIDO PINTOBASKET vs RECUCYM BAZU</t>
+        </is>
+      </c>
+    </row>
+    <row r="229">
+      <c r="A229" t="n">
+        <v>2487657</v>
+      </c>
+      <c r="B229" t="inlineStr">
+        <is>
+          <t>GRUPO EGIDO PINTOBASKET</t>
+        </is>
+      </c>
+      <c r="C229" t="inlineStr">
+        <is>
+          <t>C. BARROS CONDES | M. ALARCON ORTIZ | M. BATLLE BERNARDO | M. DEL VALLE REGALADO | S. RODRIGUEZ GREGORIO</t>
+        </is>
+      </c>
+      <c r="D229" t="n">
+        <v>5</v>
+      </c>
+      <c r="E229" t="n">
+        <v>11</v>
+      </c>
+      <c r="F229" t="n">
+        <v>0.18</v>
+      </c>
+      <c r="G229" t="n">
+        <v>0</v>
+      </c>
+      <c r="H229" t="n">
+        <v>0</v>
+      </c>
+      <c r="I229" t="n">
+        <v>0</v>
+      </c>
+      <c r="J229" t="n">
+        <v>0</v>
+      </c>
+      <c r="K229" t="inlineStr"/>
+      <c r="L229" t="inlineStr"/>
+      <c r="M229" t="inlineStr"/>
+      <c r="N229" t="n">
+        <v>0</v>
+      </c>
+      <c r="O229" t="n">
+        <v>0</v>
+      </c>
+      <c r="P229" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q229" t="n">
+        <v>0</v>
+      </c>
+      <c r="R229" t="n">
+        <v>0</v>
+      </c>
+      <c r="S229" t="n">
+        <v>0</v>
+      </c>
+      <c r="T229" t="n">
+        <v>0</v>
+      </c>
+      <c r="U229" t="n">
+        <v>0</v>
+      </c>
+      <c r="V229" t="inlineStr">
+        <is>
+          <t>Liga Regular "B-B"</t>
+        </is>
+      </c>
+      <c r="W229" t="n">
+        <v>12</v>
+      </c>
+      <c r="X229" t="inlineStr">
+        <is>
+          <t>GRUPO EGIDO PINTOBASKET vs RECUCYM BAZU</t>
+        </is>
+      </c>
+    </row>
+    <row r="230">
+      <c r="A230" t="n">
+        <v>2487657</v>
+      </c>
+      <c r="B230" t="inlineStr">
+        <is>
+          <t>GRUPO EGIDO PINTOBASKET</t>
+        </is>
+      </c>
+      <c r="C230" t="inlineStr">
+        <is>
+          <t>D. TOLOSA OROPESA | L. BERMEJO ALCALDE | M. DEL VALLE REGALADO | S. RODRIGUEZ GREGORIO</t>
+        </is>
+      </c>
+      <c r="D230" t="n">
+        <v>4</v>
+      </c>
+      <c r="E230" t="n">
+        <v>19</v>
+      </c>
+      <c r="F230" t="n">
+        <v>0.32</v>
+      </c>
+      <c r="G230" t="n">
+        <v>3</v>
+      </c>
+      <c r="H230" t="n">
+        <v>2</v>
+      </c>
+      <c r="I230" t="n">
+        <v>1.32</v>
+      </c>
+      <c r="J230" t="n">
+        <v>1</v>
+      </c>
+      <c r="K230" t="n">
+        <v>227.27</v>
+      </c>
+      <c r="L230" t="n">
+        <v>200</v>
+      </c>
+      <c r="M230" t="n">
+        <v>27.27</v>
+      </c>
+      <c r="N230" t="n">
+        <v>0</v>
+      </c>
+      <c r="O230" t="n">
+        <v>3</v>
+      </c>
+      <c r="P230" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q230" t="n">
+        <v>0</v>
+      </c>
+      <c r="R230" t="n">
+        <v>1</v>
+      </c>
+      <c r="S230" t="n">
+        <v>0</v>
+      </c>
+      <c r="T230" t="n">
+        <v>0</v>
+      </c>
+      <c r="U230" t="n">
+        <v>0</v>
+      </c>
+      <c r="V230" t="inlineStr">
+        <is>
+          <t>Liga Regular "B-B"</t>
+        </is>
+      </c>
+      <c r="W230" t="n">
+        <v>12</v>
+      </c>
+      <c r="X230" t="inlineStr">
+        <is>
+          <t>GRUPO EGIDO PINTOBASKET vs RECUCYM BAZU</t>
+        </is>
+      </c>
+    </row>
+    <row r="231">
+      <c r="A231" t="n">
+        <v>2487657</v>
+      </c>
+      <c r="B231" t="inlineStr">
+        <is>
+          <t>RECUCYM BAZU</t>
+        </is>
+      </c>
+      <c r="C231" t="inlineStr">
+        <is>
+          <t>E. ECHEVERRIA MATEO | J. BARRA DE LA CRUZ | J. MUNRO | L. DE LA CRUZ DE LA ROSA | M. OILLATAGUERRE</t>
+        </is>
+      </c>
+      <c r="D231" t="n">
+        <v>5</v>
+      </c>
+      <c r="E231" t="n">
+        <v>466</v>
+      </c>
+      <c r="F231" t="n">
+        <v>7.77</v>
+      </c>
+      <c r="G231" t="n">
+        <v>20</v>
+      </c>
+      <c r="H231" t="n">
+        <v>12</v>
+      </c>
+      <c r="I231" t="n">
+        <v>17.64</v>
+      </c>
+      <c r="J231" t="n">
+        <v>18.08</v>
+      </c>
+      <c r="K231" t="n">
+        <v>113.38</v>
+      </c>
+      <c r="L231" t="n">
+        <v>66.37</v>
+      </c>
+      <c r="M231" t="n">
+        <v>47.01</v>
+      </c>
+      <c r="N231" t="n">
+        <v>14</v>
+      </c>
+      <c r="O231" t="n">
+        <v>6</v>
+      </c>
+      <c r="P231" t="n">
+        <v>5</v>
+      </c>
+      <c r="Q231" t="n">
+        <v>4</v>
+      </c>
+      <c r="R231" t="n">
+        <v>13</v>
+      </c>
+      <c r="S231" t="n">
+        <v>7</v>
+      </c>
+      <c r="T231" t="n">
+        <v>3</v>
+      </c>
+      <c r="U231" t="n">
+        <v>1</v>
+      </c>
+      <c r="V231" t="inlineStr">
+        <is>
+          <t>Liga Regular "B-B"</t>
+        </is>
+      </c>
+      <c r="W231" t="n">
+        <v>12</v>
+      </c>
+      <c r="X231" t="inlineStr">
+        <is>
+          <t>GRUPO EGIDO PINTOBASKET vs RECUCYM BAZU</t>
+        </is>
+      </c>
+    </row>
+    <row r="232">
+      <c r="A232" t="n">
+        <v>2487654</v>
+      </c>
+      <c r="B232" t="inlineStr">
+        <is>
+          <t>BALONCESTO TALAVERA</t>
+        </is>
+      </c>
+      <c r="C232" t="inlineStr">
+        <is>
+          <t>B. GUEYE | C. KLOTZ MAROTO | C. UNANUE CEGARRA | D. LORENZO NEGRETE | V. ALONSO PASCUAL</t>
+        </is>
+      </c>
+      <c r="D232" t="n">
+        <v>5</v>
+      </c>
+      <c r="E232" t="n">
+        <v>85</v>
+      </c>
+      <c r="F232" t="n">
+        <v>1.42</v>
+      </c>
+      <c r="G232" t="n">
+        <v>7</v>
+      </c>
+      <c r="H232" t="n">
+        <v>1</v>
+      </c>
+      <c r="I232" t="n">
+        <v>2.88</v>
+      </c>
+      <c r="J232" t="n">
+        <v>2.88</v>
+      </c>
+      <c r="K232" t="n">
+        <v>243.06</v>
+      </c>
+      <c r="L232" t="n">
+        <v>34.72</v>
+      </c>
+      <c r="M232" t="n">
+        <v>208.33</v>
+      </c>
+      <c r="N232" t="n">
+        <v>2</v>
+      </c>
+      <c r="O232" t="n">
+        <v>2</v>
+      </c>
+      <c r="P232" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q232" t="n">
+        <v>0</v>
+      </c>
+      <c r="R232" t="n">
+        <v>0</v>
+      </c>
+      <c r="S232" t="n">
+        <v>2</v>
+      </c>
+      <c r="T232" t="n">
+        <v>2</v>
+      </c>
+      <c r="U232" t="n">
+        <v>0</v>
+      </c>
+      <c r="V232" t="inlineStr">
+        <is>
+          <t>Liga Regular "B-B"</t>
+        </is>
+      </c>
+      <c r="W232" t="n">
+        <v>12</v>
+      </c>
+      <c r="X232" t="inlineStr">
+        <is>
+          <t>BALONCESTO TALAVERA vs CB ARIDANE</t>
+        </is>
+      </c>
+    </row>
+    <row r="233">
+      <c r="A233" t="n">
+        <v>2487654</v>
+      </c>
+      <c r="B233" t="inlineStr">
+        <is>
+          <t>BALONCESTO TALAVERA</t>
+        </is>
+      </c>
+      <c r="C233" t="inlineStr">
+        <is>
+          <t>C. UNANUE CEGARRA | D. LORENZO NEGRETE | J. FRANCES PASCUAL | S. GACIC | V. ALONSO PASCUAL</t>
+        </is>
+      </c>
+      <c r="D233" t="n">
+        <v>5</v>
+      </c>
+      <c r="E233" t="n">
+        <v>58</v>
+      </c>
+      <c r="F233" t="n">
+        <v>0.97</v>
+      </c>
+      <c r="G233" t="n">
+        <v>2</v>
+      </c>
+      <c r="H233" t="n">
+        <v>2</v>
+      </c>
+      <c r="I233" t="n">
+        <v>2.44</v>
+      </c>
+      <c r="J233" t="n">
+        <v>0</v>
+      </c>
+      <c r="K233" t="n">
+        <v>81.97</v>
+      </c>
+      <c r="L233" t="inlineStr"/>
+      <c r="M233" t="inlineStr"/>
+      <c r="N233" t="n">
+        <v>1</v>
+      </c>
+      <c r="O233" t="n">
+        <v>1</v>
+      </c>
+      <c r="P233" t="n">
+        <v>1</v>
+      </c>
+      <c r="Q233" t="n">
+        <v>0</v>
+      </c>
+      <c r="R233" t="n">
+        <v>1</v>
+      </c>
+      <c r="S233" t="n">
+        <v>0</v>
+      </c>
+      <c r="T233" t="n">
+        <v>0</v>
+      </c>
+      <c r="U233" t="n">
+        <v>1</v>
+      </c>
+      <c r="V233" t="inlineStr">
+        <is>
+          <t>Liga Regular "B-B"</t>
+        </is>
+      </c>
+      <c r="W233" t="n">
+        <v>12</v>
+      </c>
+      <c r="X233" t="inlineStr">
+        <is>
+          <t>BALONCESTO TALAVERA vs CB ARIDANE</t>
+        </is>
+      </c>
+    </row>
+    <row r="234">
+      <c r="A234" t="n">
+        <v>2487654</v>
+      </c>
+      <c r="B234" t="inlineStr">
+        <is>
+          <t>BALONCESTO TALAVERA</t>
+        </is>
+      </c>
+      <c r="C234" t="inlineStr">
+        <is>
+          <t>C. KLOTZ MAROTO | C. UNANUE CEGARRA | J. FRANCES PASCUAL | S. GACIC | V. ALONSO PASCUAL</t>
+        </is>
+      </c>
+      <c r="D234" t="n">
+        <v>5</v>
+      </c>
+      <c r="E234" t="n">
+        <v>47</v>
+      </c>
+      <c r="F234" t="n">
+        <v>0.78</v>
+      </c>
+      <c r="G234" t="n">
+        <v>2</v>
+      </c>
+      <c r="H234" t="n">
+        <v>1</v>
+      </c>
+      <c r="I234" t="n">
+        <v>0.88</v>
+      </c>
+      <c r="J234" t="n">
+        <v>1.88</v>
+      </c>
+      <c r="K234" t="n">
+        <v>227.27</v>
+      </c>
+      <c r="L234" t="n">
+        <v>53.19</v>
+      </c>
+      <c r="M234" t="n">
+        <v>174.08</v>
+      </c>
+      <c r="N234" t="n">
+        <v>1</v>
+      </c>
+      <c r="O234" t="n">
+        <v>2</v>
+      </c>
+      <c r="P234" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q234" t="n">
+        <v>1</v>
+      </c>
+      <c r="R234" t="n">
+        <v>1</v>
+      </c>
+      <c r="S234" t="n">
+        <v>2</v>
+      </c>
+      <c r="T234" t="n">
+        <v>0</v>
+      </c>
+      <c r="U234" t="n">
+        <v>0</v>
+      </c>
+      <c r="V234" t="inlineStr">
+        <is>
+          <t>Liga Regular "B-B"</t>
+        </is>
+      </c>
+      <c r="W234" t="n">
+        <v>12</v>
+      </c>
+      <c r="X234" t="inlineStr">
+        <is>
+          <t>BALONCESTO TALAVERA vs CB ARIDANE</t>
+        </is>
+      </c>
+    </row>
+    <row r="235">
+      <c r="A235" t="n">
+        <v>2487654</v>
+      </c>
+      <c r="B235" t="inlineStr">
+        <is>
+          <t>BALONCESTO TALAVERA</t>
+        </is>
+      </c>
+      <c r="C235" t="inlineStr">
+        <is>
+          <t>C. KLOTZ MAROTO | C. UNANUE CEGARRA | D. LORENZO NEGRETE | J. FRANCES PASCUAL | S. GACIC</t>
+        </is>
+      </c>
+      <c r="D235" t="n">
+        <v>5</v>
+      </c>
+      <c r="E235" t="n">
+        <v>32</v>
+      </c>
+      <c r="F235" t="n">
+        <v>0.53</v>
+      </c>
+      <c r="G235" t="n">
+        <v>0</v>
+      </c>
+      <c r="H235" t="n">
+        <v>0</v>
+      </c>
+      <c r="I235" t="n">
+        <v>1</v>
+      </c>
+      <c r="J235" t="n">
+        <v>1</v>
+      </c>
+      <c r="K235" t="n">
+        <v>0</v>
+      </c>
+      <c r="L235" t="n">
+        <v>0</v>
+      </c>
+      <c r="M235" t="n">
+        <v>0</v>
+      </c>
+      <c r="N235" t="n">
+        <v>0</v>
+      </c>
+      <c r="O235" t="n">
+        <v>0</v>
+      </c>
+      <c r="P235" t="n">
+        <v>1</v>
+      </c>
+      <c r="Q235" t="n">
+        <v>0</v>
+      </c>
+      <c r="R235" t="n">
+        <v>0</v>
+      </c>
+      <c r="S235" t="n">
+        <v>0</v>
+      </c>
+      <c r="T235" t="n">
+        <v>1</v>
+      </c>
+      <c r="U235" t="n">
+        <v>0</v>
+      </c>
+      <c r="V235" t="inlineStr">
+        <is>
+          <t>Liga Regular "B-B"</t>
+        </is>
+      </c>
+      <c r="W235" t="n">
+        <v>12</v>
+      </c>
+      <c r="X235" t="inlineStr">
+        <is>
+          <t>BALONCESTO TALAVERA vs CB ARIDANE</t>
+        </is>
+      </c>
+    </row>
+    <row r="236">
+      <c r="A236" t="n">
+        <v>2487654</v>
+      </c>
+      <c r="B236" t="inlineStr">
+        <is>
+          <t>CB ARIDANE</t>
+        </is>
+      </c>
+      <c r="C236" t="inlineStr">
+        <is>
+          <t>D. VIERA LOPEZ | E. LLACER SIMLAT | J. ABRIL RAMIRO | O. BALSELLS PLAZA | S. GUEYE</t>
+        </is>
+      </c>
+      <c r="D236" t="n">
+        <v>5</v>
+      </c>
+      <c r="E236" t="n">
+        <v>126</v>
+      </c>
+      <c r="F236" t="n">
+        <v>2.1</v>
+      </c>
+      <c r="G236" t="n">
+        <v>1</v>
+      </c>
+      <c r="H236" t="n">
+        <v>6</v>
+      </c>
+      <c r="I236" t="n">
+        <v>4.88</v>
+      </c>
+      <c r="J236" t="n">
+        <v>3.76</v>
+      </c>
+      <c r="K236" t="n">
+        <v>20.49</v>
+      </c>
+      <c r="L236" t="n">
+        <v>159.57</v>
+      </c>
+      <c r="M236" t="n">
+        <v>-139.08</v>
+      </c>
+      <c r="N236" t="n">
+        <v>1</v>
+      </c>
+      <c r="O236" t="n">
+        <v>2</v>
+      </c>
+      <c r="P236" t="n">
+        <v>3</v>
+      </c>
+      <c r="Q236" t="n">
+        <v>0</v>
+      </c>
+      <c r="R236" t="n">
+        <v>2</v>
+      </c>
+      <c r="S236" t="n">
+        <v>4</v>
+      </c>
+      <c r="T236" t="n">
+        <v>1</v>
+      </c>
+      <c r="U236" t="n">
+        <v>1</v>
+      </c>
+      <c r="V236" t="inlineStr">
+        <is>
+          <t>Liga Regular "B-B"</t>
+        </is>
+      </c>
+      <c r="W236" t="n">
+        <v>12</v>
+      </c>
+      <c r="X236" t="inlineStr">
+        <is>
+          <t>BALONCESTO TALAVERA vs CB ARIDANE</t>
+        </is>
+      </c>
+    </row>
+    <row r="237">
+      <c r="A237" t="n">
+        <v>2487654</v>
+      </c>
+      <c r="B237" t="inlineStr">
+        <is>
+          <t>CB ARIDANE</t>
+        </is>
+      </c>
+      <c r="C237" t="inlineStr">
+        <is>
+          <t>D. VIERA LOPEZ | E. LLACER SIMLAT | K. SKUTYELNIK | O. BALSELLS PLAZA | S. GUEYE</t>
+        </is>
+      </c>
+      <c r="D237" t="n">
+        <v>5</v>
+      </c>
+      <c r="E237" t="n">
+        <v>96</v>
+      </c>
+      <c r="F237" t="n">
+        <v>1.6</v>
+      </c>
+      <c r="G237" t="n">
+        <v>3</v>
+      </c>
+      <c r="H237" t="n">
+        <v>5</v>
+      </c>
+      <c r="I237" t="n">
+        <v>0.88</v>
+      </c>
+      <c r="J237" t="n">
+        <v>3.44</v>
+      </c>
+      <c r="K237" t="n">
+        <v>340.91</v>
+      </c>
+      <c r="L237" t="n">
+        <v>145.35</v>
+      </c>
+      <c r="M237" t="n">
+        <v>195.56</v>
+      </c>
+      <c r="N237" t="n">
+        <v>1</v>
+      </c>
+      <c r="O237" t="n">
+        <v>2</v>
+      </c>
+      <c r="P237" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q237" t="n">
+        <v>1</v>
+      </c>
+      <c r="R237" t="n">
+        <v>2</v>
+      </c>
+      <c r="S237" t="n">
+        <v>1</v>
+      </c>
+      <c r="T237" t="n">
+        <v>1</v>
+      </c>
+      <c r="U237" t="n">
+        <v>0</v>
+      </c>
+      <c r="V237" t="inlineStr">
+        <is>
+          <t>Liga Regular "B-B"</t>
+        </is>
+      </c>
+      <c r="W237" t="n">
+        <v>12</v>
+      </c>
+      <c r="X237" t="inlineStr">
+        <is>
+          <t>BALONCESTO TALAVERA vs CB ARIDANE</t>
+        </is>
+      </c>
+    </row>
+    <row r="238">
+      <c r="A238" t="n">
+        <v>2487659</v>
+      </c>
+      <c r="B238" t="inlineStr">
+        <is>
+          <t>C.B. TRES CANTOS</t>
+        </is>
+      </c>
+      <c r="C238" t="inlineStr">
+        <is>
+          <t>D. FERNANDEZ CAÑAS | G. DIAZ MONTERO | H. PEREZ SANCHEZ | J. ATIENZA PEREA | N. MAIGA</t>
+        </is>
+      </c>
+      <c r="D238" t="n">
+        <v>5</v>
+      </c>
+      <c r="E238" t="n">
+        <v>175</v>
+      </c>
+      <c r="F238" t="n">
+        <v>2.92</v>
+      </c>
+      <c r="G238" t="n">
+        <v>7</v>
+      </c>
+      <c r="H238" t="n">
+        <v>2</v>
+      </c>
+      <c r="I238" t="n">
+        <v>5.76</v>
+      </c>
+      <c r="J238" t="n">
+        <v>7.76</v>
+      </c>
+      <c r="K238" t="n">
+        <v>121.53</v>
+      </c>
+      <c r="L238" t="n">
+        <v>25.77</v>
+      </c>
+      <c r="M238" t="n">
+        <v>95.75</v>
+      </c>
+      <c r="N238" t="n">
+        <v>6</v>
+      </c>
+      <c r="O238" t="n">
+        <v>4</v>
+      </c>
+      <c r="P238" t="n">
+        <v>1</v>
+      </c>
+      <c r="Q238" t="n">
+        <v>3</v>
+      </c>
+      <c r="R238" t="n">
+        <v>7</v>
+      </c>
+      <c r="S238" t="n">
+        <v>4</v>
+      </c>
+      <c r="T238" t="n">
+        <v>1</v>
+      </c>
+      <c r="U238" t="n">
+        <v>2</v>
+      </c>
+      <c r="V238" t="inlineStr">
+        <is>
+          <t>Liga Regular "B-B"</t>
+        </is>
+      </c>
+      <c r="W238" t="n">
+        <v>12</v>
+      </c>
+      <c r="X238" t="inlineStr">
+        <is>
+          <t>C.B. TRES CANTOS vs ZENTRO BASKET MADRID</t>
+        </is>
+      </c>
+    </row>
+    <row r="239">
+      <c r="A239" t="n">
+        <v>2487659</v>
+      </c>
+      <c r="B239" t="inlineStr">
+        <is>
+          <t>C.B. TRES CANTOS</t>
+        </is>
+      </c>
+      <c r="C239" t="inlineStr">
+        <is>
+          <t>D. FERNANDEZ CAÑAS | G. DIAZ MONTERO | J. ATIENZA PEREA | N. MAIGA</t>
+        </is>
+      </c>
+      <c r="D239" t="n">
+        <v>4</v>
+      </c>
+      <c r="E239" t="n">
+        <v>13</v>
+      </c>
+      <c r="F239" t="n">
+        <v>0.22</v>
+      </c>
+      <c r="G239" t="n">
+        <v>2</v>
+      </c>
+      <c r="H239" t="n">
+        <v>0</v>
+      </c>
+      <c r="I239" t="n">
+        <v>1</v>
+      </c>
+      <c r="J239" t="n">
+        <v>0</v>
+      </c>
+      <c r="K239" t="n">
+        <v>200</v>
+      </c>
+      <c r="L239" t="inlineStr"/>
+      <c r="M239" t="inlineStr"/>
+      <c r="N239" t="n">
+        <v>1</v>
+      </c>
+      <c r="O239" t="n">
+        <v>0</v>
+      </c>
+      <c r="P239" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q239" t="n">
+        <v>0</v>
+      </c>
+      <c r="R239" t="n">
+        <v>1</v>
+      </c>
+      <c r="S239" t="n">
+        <v>0</v>
+      </c>
+      <c r="T239" t="n">
+        <v>0</v>
+      </c>
+      <c r="U239" t="n">
+        <v>1</v>
+      </c>
+      <c r="V239" t="inlineStr">
+        <is>
+          <t>Liga Regular "B-B"</t>
+        </is>
+      </c>
+      <c r="W239" t="n">
+        <v>12</v>
+      </c>
+      <c r="X239" t="inlineStr">
+        <is>
+          <t>C.B. TRES CANTOS vs ZENTRO BASKET MADRID</t>
+        </is>
+      </c>
+    </row>
+    <row r="240">
+      <c r="A240" t="n">
+        <v>2487659</v>
+      </c>
+      <c r="B240" t="inlineStr">
+        <is>
+          <t>ZENTRO BASKET MADRID</t>
+        </is>
+      </c>
+      <c r="C240" t="inlineStr">
+        <is>
+          <t>B. SCHUCH | G. GOMA | J. VAQUERO PASCUAL | L. SCHIEBELHUT LUIS | M. ESTAPE ROIZ | M. RUBIO CORCHADO</t>
+        </is>
+      </c>
+      <c r="D240" t="n">
+        <v>6</v>
+      </c>
+      <c r="E240" t="n">
+        <v>7</v>
+      </c>
+      <c r="F240" t="n">
+        <v>0.12</v>
+      </c>
+      <c r="G240" t="n">
+        <v>0</v>
+      </c>
+      <c r="H240" t="n">
+        <v>2</v>
+      </c>
+      <c r="I240" t="n">
+        <v>1</v>
+      </c>
+      <c r="J240" t="n">
+        <v>0.76</v>
+      </c>
+      <c r="K240" t="n">
+        <v>0</v>
+      </c>
+      <c r="L240" t="n">
+        <v>263.16</v>
+      </c>
+      <c r="M240" t="n">
+        <v>-263.16</v>
+      </c>
+      <c r="N240" t="n">
+        <v>2</v>
+      </c>
+      <c r="O240" t="n">
+        <v>0</v>
+      </c>
+      <c r="P240" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q240" t="n">
+        <v>1</v>
+      </c>
+      <c r="R240" t="n">
+        <v>0</v>
+      </c>
+      <c r="S240" t="n">
+        <v>4</v>
+      </c>
+      <c r="T240" t="n">
+        <v>0</v>
+      </c>
+      <c r="U240" t="n">
+        <v>1</v>
+      </c>
+      <c r="V240" t="inlineStr">
+        <is>
+          <t>Liga Regular "B-B"</t>
+        </is>
+      </c>
+      <c r="W240" t="n">
+        <v>12</v>
+      </c>
+      <c r="X240" t="inlineStr">
+        <is>
+          <t>C.B. TRES CANTOS vs ZENTRO BASKET MADRID</t>
+        </is>
+      </c>
+    </row>
+    <row r="241">
+      <c r="A241" t="n">
+        <v>2487659</v>
+      </c>
+      <c r="B241" t="inlineStr">
+        <is>
+          <t>ZENTRO BASKET MADRID</t>
+        </is>
+      </c>
+      <c r="C241" t="inlineStr">
+        <is>
+          <t>B. SCHUCH | G. GOMA | L. SCHIEBELHUT LUIS | M. RUBIO CORCHADO | T. VERDERA BENASSAR</t>
+        </is>
+      </c>
+      <c r="D241" t="n">
+        <v>5</v>
+      </c>
+      <c r="E241" t="n">
+        <v>109</v>
+      </c>
+      <c r="F241" t="n">
+        <v>1.82</v>
+      </c>
+      <c r="G241" t="n">
+        <v>2</v>
+      </c>
+      <c r="H241" t="n">
+        <v>3</v>
+      </c>
+      <c r="I241" t="n">
+        <v>3.88</v>
+      </c>
+      <c r="J241" t="n">
+        <v>3</v>
+      </c>
+      <c r="K241" t="n">
+        <v>51.55</v>
+      </c>
+      <c r="L241" t="n">
+        <v>100</v>
+      </c>
+      <c r="M241" t="n">
+        <v>-48.45</v>
+      </c>
+      <c r="N241" t="n">
+        <v>4</v>
+      </c>
+      <c r="O241" t="n">
+        <v>2</v>
+      </c>
+      <c r="P241" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q241" t="n">
+        <v>1</v>
+      </c>
+      <c r="R241" t="n">
+        <v>4</v>
+      </c>
+      <c r="S241" t="n">
+        <v>0</v>
+      </c>
+      <c r="T241" t="n">
+        <v>0</v>
+      </c>
+      <c r="U241" t="n">
+        <v>1</v>
+      </c>
+      <c r="V241" t="inlineStr">
+        <is>
+          <t>Liga Regular "B-B"</t>
+        </is>
+      </c>
+      <c r="W241" t="n">
+        <v>12</v>
+      </c>
+      <c r="X241" t="inlineStr">
+        <is>
+          <t>C.B. TRES CANTOS vs ZENTRO BASKET MADRID</t>
+        </is>
+      </c>
+    </row>
+    <row r="242">
+      <c r="A242" t="n">
+        <v>2487659</v>
+      </c>
+      <c r="B242" t="inlineStr">
+        <is>
+          <t>ZENTRO BASKET MADRID</t>
+        </is>
+      </c>
+      <c r="C242" t="inlineStr">
+        <is>
+          <t>B. SCHUCH | G. GOMA | J. VAQUERO PASCUAL | L. SCHIEBELHUT LUIS | M. RUBIO CORCHADO</t>
+        </is>
+      </c>
+      <c r="D242" t="n">
+        <v>5</v>
+      </c>
+      <c r="E242" t="n">
+        <v>43</v>
+      </c>
+      <c r="F242" t="n">
+        <v>0.72</v>
+      </c>
+      <c r="G242" t="n">
+        <v>0</v>
+      </c>
+      <c r="H242" t="n">
+        <v>2</v>
+      </c>
+      <c r="I242" t="n">
+        <v>1</v>
+      </c>
+      <c r="J242" t="n">
+        <v>1</v>
+      </c>
+      <c r="K242" t="n">
+        <v>0</v>
+      </c>
+      <c r="L242" t="n">
+        <v>200</v>
+      </c>
+      <c r="M242" t="n">
+        <v>-200</v>
+      </c>
+      <c r="N242" t="n">
+        <v>0</v>
+      </c>
+      <c r="O242" t="n">
+        <v>0</v>
+      </c>
+      <c r="P242" t="n">
+        <v>1</v>
+      </c>
+      <c r="Q242" t="n">
+        <v>0</v>
+      </c>
+      <c r="R242" t="n">
+        <v>2</v>
+      </c>
+      <c r="S242" t="n">
+        <v>0</v>
+      </c>
+      <c r="T242" t="n">
+        <v>0</v>
+      </c>
+      <c r="U242" t="n">
+        <v>1</v>
+      </c>
+      <c r="V242" t="inlineStr">
+        <is>
+          <t>Liga Regular "B-B"</t>
+        </is>
+      </c>
+      <c r="W242" t="n">
+        <v>12</v>
+      </c>
+      <c r="X242" t="inlineStr">
+        <is>
+          <t>C.B. TRES CANTOS vs ZENTRO BASKET MADRID</t>
+        </is>
+      </c>
+    </row>
+    <row r="243">
+      <c r="A243" t="n">
+        <v>2487659</v>
+      </c>
+      <c r="B243" t="inlineStr">
+        <is>
+          <t>ZENTRO BASKET MADRID</t>
+        </is>
+      </c>
+      <c r="C243" t="inlineStr">
+        <is>
+          <t>B. SCHUCH | G. GOMA | J. VAQUERO PASCUAL | M. RUBIO CORCHADO | T. VERDERA BENASSAR</t>
+        </is>
+      </c>
+      <c r="D243" t="n">
+        <v>5</v>
+      </c>
+      <c r="E243" t="n">
+        <v>16</v>
+      </c>
+      <c r="F243" t="n">
+        <v>0.27</v>
+      </c>
+      <c r="G243" t="n">
+        <v>0</v>
+      </c>
+      <c r="H243" t="n">
+        <v>0</v>
+      </c>
+      <c r="I243" t="n">
+        <v>1.88</v>
+      </c>
+      <c r="J243" t="n">
+        <v>1</v>
+      </c>
+      <c r="K243" t="n">
+        <v>0</v>
+      </c>
+      <c r="L243" t="n">
+        <v>0</v>
+      </c>
+      <c r="M243" t="n">
+        <v>0</v>
+      </c>
+      <c r="N243" t="n">
+        <v>1</v>
+      </c>
+      <c r="O243" t="n">
+        <v>2</v>
+      </c>
+      <c r="P243" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q243" t="n">
+        <v>0</v>
+      </c>
+      <c r="R243" t="n">
+        <v>0</v>
+      </c>
+      <c r="S243" t="n">
+        <v>0</v>
+      </c>
+      <c r="T243" t="n">
+        <v>1</v>
+      </c>
+      <c r="U243" t="n">
+        <v>0</v>
+      </c>
+      <c r="V243" t="inlineStr">
+        <is>
+          <t>Liga Regular "B-B"</t>
+        </is>
+      </c>
+      <c r="W243" t="n">
+        <v>12</v>
+      </c>
+      <c r="X243" t="inlineStr">
+        <is>
+          <t>C.B. TRES CANTOS vs ZENTRO BASKET MADRID</t>
+        </is>
+      </c>
+    </row>
+    <row r="244">
+      <c r="A244" t="n">
+        <v>2487659</v>
+      </c>
+      <c r="B244" t="inlineStr">
+        <is>
+          <t>ZENTRO BASKET MADRID</t>
+        </is>
+      </c>
+      <c r="C244" t="inlineStr">
+        <is>
+          <t>B. SCHUCH | D. VAL GUTIERREZ | G. GOMA | J. VAQUERO PASCUAL | L. SCHIEBELHUT LUIS</t>
+        </is>
+      </c>
+      <c r="D244" t="n">
+        <v>5</v>
+      </c>
+      <c r="E244" t="n">
+        <v>13</v>
+      </c>
+      <c r="F244" t="n">
+        <v>0.22</v>
+      </c>
+      <c r="G244" t="n">
+        <v>0</v>
+      </c>
+      <c r="H244" t="n">
+        <v>2</v>
+      </c>
+      <c r="I244" t="n">
+        <v>0</v>
+      </c>
+      <c r="J244" t="n">
+        <v>1</v>
+      </c>
+      <c r="K244" t="inlineStr"/>
+      <c r="L244" t="n">
+        <v>200</v>
+      </c>
+      <c r="M244" t="inlineStr"/>
+      <c r="N244" t="n">
+        <v>1</v>
+      </c>
+      <c r="O244" t="n">
+        <v>0</v>
+      </c>
+      <c r="P244" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q244" t="n">
+        <v>1</v>
+      </c>
+      <c r="R244" t="n">
+        <v>1</v>
+      </c>
+      <c r="S244" t="n">
+        <v>0</v>
+      </c>
+      <c r="T244" t="n">
+        <v>0</v>
+      </c>
+      <c r="U244" t="n">
+        <v>0</v>
+      </c>
+      <c r="V244" t="inlineStr">
+        <is>
+          <t>Liga Regular "B-B"</t>
+        </is>
+      </c>
+      <c r="W244" t="n">
+        <v>12</v>
+      </c>
+      <c r="X244" t="inlineStr">
+        <is>
+          <t>C.B. TRES CANTOS vs ZENTRO BASKET MADRID</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>